<commit_message>
update plan data files
</commit_message>
<xml_diff>
--- a/Data_inputs/MISERS_MemberData.xlsx
+++ b/Data_inputs/MISERS_MemberData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="2" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="20" r:id="rId1"/>
@@ -15,8 +15,8 @@
     <sheet name="Actives_t1_CRR2013" sheetId="33" r:id="rId6"/>
     <sheet name="Actives_t1.num_CRR2013" sheetId="27" r:id="rId7"/>
     <sheet name="Actives_t1.sal_CRR2013" sheetId="28" r:id="rId8"/>
-    <sheet name="RetBen_CRR2013" sheetId="31" r:id="rId9"/>
-    <sheet name="RetBen_AV2014" sheetId="30" r:id="rId10"/>
+    <sheet name="RetBen_AV2014" sheetId="30" r:id="rId9"/>
+    <sheet name="RetBen_CRR2013" sheetId="31" r:id="rId10"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="106">
   <si>
     <t>TOC</t>
   </si>
@@ -318,34 +318,6 @@
         <sz val="12"/>
         <rFont val="Times New Roman"/>
       </rPr>
-      <t xml:space="preserve">Total
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>Pay</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
       <t xml:space="preserve">Average
 </t>
     </r>
@@ -563,6 +535,18 @@
   <si>
     <t>other</t>
   </si>
+  <si>
+    <t>salary.avg</t>
+  </si>
+  <si>
+    <t>L18</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>female</t>
+  </si>
 </sst>
 </file>
 
@@ -571,7 +555,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0;&quot;$&quot;\-#,##0"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -617,12 +601,6 @@
       <name val="Times New Roman"/>
     </font>
     <font>
-      <b/>
-      <vertAlign val="superscript"/>
-      <sz val="12"/>
-      <name val="Times New Roman"/>
-    </font>
-    <font>
       <sz val="12"/>
       <name val="Times New Roman"/>
     </font>
@@ -653,7 +631,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -724,12 +702,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -749,79 +736,97 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" indent="2"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1" indent="3"/>
+    <xf numFmtId="3" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="3"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -844,16 +849,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>952500</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>933450</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>256070</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>151736</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>8420</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>189836</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -870,7 +875,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8991600" y="1600200"/>
+          <a:off x="7391400" y="4543425"/>
           <a:ext cx="8838095" cy="5314286"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1013,6 +1018,49 @@
 </file>
 
 <file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>27706</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>170305</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5772150" y="533400"/>
+          <a:ext cx="6952381" cy="9161905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1193,49 +1241,6 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>380131</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>56005</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1104900" y="609600"/>
-          <a:ext cx="6952381" cy="9161905"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1724,20 +1729,21 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="O28" sqref="O28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="10" max="10" width="18.28515625" customWidth="1"/>
-    <col min="11" max="13" width="14.5703125" customWidth="1"/>
-    <col min="14" max="14" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="9.140625" customWidth="1"/>
+    <col min="12" max="12" width="18.28515625" customWidth="1"/>
+    <col min="13" max="15" width="14.5703125" customWidth="1"/>
+    <col min="16" max="16" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1750,13 +1756,17 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
-      <c r="N1" s="1"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="P1" s="1"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -1765,13 +1775,17 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
-      <c r="N2" s="2"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="P2" s="2"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>98</v>
+      </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -1780,14 +1794,293 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
-      <c r="N3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="P3" s="2"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="29">
+        <v>27</v>
+      </c>
+      <c r="D6" s="29">
+        <v>533</v>
+      </c>
+      <c r="E6" s="29">
+        <f>F6/D6</f>
+        <v>1615.7913193245779</v>
+      </c>
+      <c r="F6">
+        <v>861216.77320000005</v>
+      </c>
+      <c r="G6">
+        <f>E6*12</f>
+        <v>19389.495831894936</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="29">
+        <v>32</v>
+      </c>
+      <c r="D7" s="29">
+        <v>1010</v>
+      </c>
+      <c r="E7" s="29">
+        <f t="shared" ref="E7:E17" si="0">F7/D7</f>
+        <v>1615.7913198019803</v>
+      </c>
+      <c r="F7">
+        <v>1631949.233</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="29">
+        <v>37</v>
+      </c>
+      <c r="D8" s="29">
+        <v>3503</v>
+      </c>
+      <c r="E8" s="29">
+        <f t="shared" si="0"/>
+        <v>1615.7913194404796</v>
+      </c>
+      <c r="F8">
+        <v>5660116.9919999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="29">
+        <v>42</v>
+      </c>
+      <c r="D9" s="29">
+        <v>7419</v>
+      </c>
+      <c r="E9" s="29">
+        <f t="shared" si="0"/>
+        <v>1615.7913195848498</v>
+      </c>
+      <c r="F9">
+        <v>11987555.800000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="29">
+        <v>47</v>
+      </c>
+      <c r="D10" s="29">
+        <v>6631</v>
+      </c>
+      <c r="E10" s="29">
+        <f t="shared" si="0"/>
+        <v>1615.7913195596441</v>
+      </c>
+      <c r="F10">
+        <v>10714312.24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="29">
+        <v>52</v>
+      </c>
+      <c r="D11" s="29">
+        <v>4813</v>
+      </c>
+      <c r="E11" s="29">
+        <f t="shared" si="0"/>
+        <v>1615.7913193434449</v>
+      </c>
+      <c r="F11">
+        <v>7776803.6200000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="29">
+        <v>57</v>
+      </c>
+      <c r="D12" s="29">
+        <v>3457</v>
+      </c>
+      <c r="E12" s="29">
+        <f t="shared" si="0"/>
+        <v>1615.7913193520394</v>
+      </c>
+      <c r="F12">
+        <v>5585790.591</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="29">
+        <v>62</v>
+      </c>
+      <c r="D13" s="29">
+        <v>2455</v>
+      </c>
+      <c r="E13" s="29">
+        <f t="shared" si="0"/>
+        <v>1615.7913193482686</v>
+      </c>
+      <c r="F13">
+        <v>3966767.6889999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="29">
+        <v>67</v>
+      </c>
+      <c r="D14" s="29">
+        <v>1626</v>
+      </c>
+      <c r="E14" s="29">
+        <f t="shared" si="0"/>
+        <v>1615.7913191881919</v>
+      </c>
+      <c r="F14">
+        <v>2627276.6850000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="29">
+        <v>72</v>
+      </c>
+      <c r="D15" s="29">
+        <v>731</v>
+      </c>
+      <c r="E15" s="29">
+        <f t="shared" si="0"/>
+        <v>1615.7913187414499</v>
+      </c>
+      <c r="F15">
+        <v>1181143.4539999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" s="29">
+        <v>77</v>
+      </c>
+      <c r="D16" s="29">
+        <v>201</v>
+      </c>
+      <c r="E16" s="29">
+        <f t="shared" si="0"/>
+        <v>1615.791319402985</v>
+      </c>
+      <c r="F16">
+        <v>324774.0552</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>5</v>
+      </c>
+      <c r="B17" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" s="29">
+        <v>82</v>
+      </c>
+      <c r="D17" s="29">
+        <v>15</v>
+      </c>
+      <c r="E17" s="29">
+        <f t="shared" si="0"/>
+        <v>1615.7913193333334</v>
+      </c>
+      <c r="F17">
+        <v>24236.869790000001</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" location="TOC!A1" display="TOC"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1795,8 +2088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1831,13 +2124,13 @@
         <v>61</v>
       </c>
       <c r="C6" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D6" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="E6" s="9" t="s">
         <v>101</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>102</v>
       </c>
       <c r="F6" s="9" t="s">
         <v>64</v>
@@ -1907,14 +2200,75 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="4" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="9">
+        <v>55</v>
+      </c>
+      <c r="D7" s="9">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="9">
+        <v>55</v>
+      </c>
+      <c r="D8" s="9">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" location="TOC!A1" display="TOC"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1924,7 +2278,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1935,20 +2289,21 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N18"/>
+  <dimension ref="A1:Y19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="10" max="10" width="18.28515625" customWidth="1"/>
-    <col min="11" max="13" width="14.5703125" customWidth="1"/>
-    <col min="14" max="14" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="14.5703125" customWidth="1"/>
+    <col min="13" max="13" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.28515625" customWidth="1"/>
+    <col min="25" max="25" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1960,14 +2315,15 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="N1" s="1"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M1" s="1"/>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -1975,14 +2331,15 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="N2" s="2"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M2" s="2"/>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>103</v>
+      </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -1990,427 +2347,793 @@
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="N3" s="2"/>
-    </row>
-    <row r="6" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="M3" s="2"/>
+    </row>
+    <row r="6" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="43">
+        <v>2</v>
+      </c>
+      <c r="F6" s="43">
+        <v>7</v>
+      </c>
+      <c r="G6" s="43">
+        <v>12</v>
+      </c>
+      <c r="H6" s="43">
+        <v>17</v>
+      </c>
+      <c r="I6" s="43">
+        <v>22</v>
+      </c>
+      <c r="J6" s="43">
+        <v>27</v>
+      </c>
+      <c r="K6" s="43">
+        <v>32</v>
+      </c>
+      <c r="L6" s="42" t="s">
+        <v>102</v>
+      </c>
+      <c r="P6" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="Q6" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11" t="s">
+      <c r="R6" s="32"/>
+      <c r="S6" s="32"/>
+      <c r="T6" s="32"/>
+      <c r="U6" s="32"/>
+      <c r="V6" s="32"/>
+      <c r="W6" s="32"/>
+      <c r="X6" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="J6" s="12" t="s">
+      <c r="Y6" s="32" t="s">
         <v>75</v>
       </c>
-      <c r="K6" s="11" t="s">
+    </row>
+    <row r="7" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="H7" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="J7" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="K7" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="L7" s="36"/>
+      <c r="P7" s="31"/>
+      <c r="Q7" s="10" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
-      <c r="B7" s="13" t="s">
+      <c r="R7" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="S7" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="T7" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="U7" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="V7" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="W7" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="H7" s="13" t="s">
+      <c r="X7" s="32"/>
+      <c r="Y7" s="32"/>
+    </row>
+    <row r="8" spans="1:25" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="33">
+        <v>22</v>
+      </c>
+      <c r="D8" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37"/>
+      <c r="J8" s="37"/>
+      <c r="K8" s="37"/>
+      <c r="L8" s="36"/>
+      <c r="P8" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="I7" s="11"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="11"/>
-    </row>
-    <row r="8" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+      <c r="Q8" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="R8" s="13"/>
+      <c r="S8" s="13"/>
+      <c r="T8" s="13"/>
+      <c r="U8" s="13"/>
+      <c r="V8" s="13"/>
+      <c r="W8" s="13"/>
+      <c r="X8" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y8" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="J8" s="15" t="s">
+    </row>
+    <row r="9" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="33">
+        <v>27</v>
+      </c>
+      <c r="D9" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="37"/>
+      <c r="J9" s="37"/>
+      <c r="K9" s="37"/>
+      <c r="L9" s="36"/>
+      <c r="P9" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="K8" s="17" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
+      <c r="Q9" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="R9" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="S9" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="T9" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="U9" s="17"/>
+      <c r="V9" s="17"/>
+      <c r="W9" s="17"/>
+      <c r="X9" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y9" s="18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="33">
+        <v>32</v>
+      </c>
+      <c r="D10" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="37"/>
+      <c r="J10" s="37"/>
+      <c r="K10" s="37"/>
+      <c r="L10" s="36"/>
+      <c r="P10" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="B9" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="C9" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="E9" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="J9" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="K9" s="21" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
+      <c r="Q10" s="19">
+        <v>7</v>
+      </c>
+      <c r="R10" s="19">
+        <v>22</v>
+      </c>
+      <c r="S10" s="19">
+        <v>27</v>
+      </c>
+      <c r="T10" s="19">
+        <v>72</v>
+      </c>
+      <c r="U10" s="19">
+        <v>12</v>
+      </c>
+      <c r="V10" s="17"/>
+      <c r="W10" s="17"/>
+      <c r="X10" s="19">
+        <v>140</v>
+      </c>
+      <c r="Y10" s="21">
+        <v>63287</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="33">
+        <v>37</v>
+      </c>
+      <c r="D11" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="38">
+        <v>7</v>
+      </c>
+      <c r="F11" s="38">
+        <v>22</v>
+      </c>
+      <c r="G11" s="38">
+        <v>27</v>
+      </c>
+      <c r="H11" s="38">
+        <v>72</v>
+      </c>
+      <c r="I11" s="38">
+        <v>12</v>
+      </c>
+      <c r="J11" s="39"/>
+      <c r="K11" s="39"/>
+      <c r="L11" s="40">
+        <v>63287</v>
+      </c>
+      <c r="P11" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="B10" s="22">
-        <v>7</v>
-      </c>
-      <c r="C10" s="22">
+      <c r="Q11" s="19">
+        <v>26</v>
+      </c>
+      <c r="R11" s="19">
+        <v>40</v>
+      </c>
+      <c r="S11" s="19">
+        <v>70</v>
+      </c>
+      <c r="T11" s="19">
+        <v>640</v>
+      </c>
+      <c r="U11" s="19">
+        <v>336</v>
+      </c>
+      <c r="V11" s="19">
+        <v>34</v>
+      </c>
+      <c r="W11" s="17"/>
+      <c r="X11" s="20">
+        <v>1146</v>
+      </c>
+      <c r="Y11" s="21">
+        <v>65611</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>5</v>
+      </c>
+      <c r="B12" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="33">
+        <v>42</v>
+      </c>
+      <c r="D12" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="38">
+        <v>26</v>
+      </c>
+      <c r="F12" s="38">
+        <v>40</v>
+      </c>
+      <c r="G12" s="38">
+        <v>70</v>
+      </c>
+      <c r="H12" s="38">
+        <v>640</v>
+      </c>
+      <c r="I12" s="38">
+        <v>336</v>
+      </c>
+      <c r="J12" s="38">
+        <v>34</v>
+      </c>
+      <c r="K12" s="39"/>
+      <c r="L12" s="40">
+        <v>65611</v>
+      </c>
+      <c r="P12" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q12" s="19">
+        <v>23</v>
+      </c>
+      <c r="R12" s="19">
+        <v>37</v>
+      </c>
+      <c r="S12" s="19">
+        <v>54</v>
+      </c>
+      <c r="T12" s="19">
+        <v>721</v>
+      </c>
+      <c r="U12" s="20">
+        <v>1066</v>
+      </c>
+      <c r="V12" s="19">
+        <v>774</v>
+      </c>
+      <c r="W12" s="19">
+        <v>73</v>
+      </c>
+      <c r="X12" s="20">
+        <v>2748</v>
+      </c>
+      <c r="Y12" s="21">
+        <v>66757</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="33">
+        <v>47</v>
+      </c>
+      <c r="D13" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="38">
+        <v>23</v>
+      </c>
+      <c r="F13" s="38">
+        <v>37</v>
+      </c>
+      <c r="G13" s="38">
+        <v>54</v>
+      </c>
+      <c r="H13" s="38">
+        <v>721</v>
+      </c>
+      <c r="I13" s="41">
+        <v>1066</v>
+      </c>
+      <c r="J13" s="38">
+        <v>774</v>
+      </c>
+      <c r="K13" s="38">
+        <v>73</v>
+      </c>
+      <c r="L13" s="40">
+        <v>66757</v>
+      </c>
+      <c r="P13" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q13" s="19">
+        <v>16</v>
+      </c>
+      <c r="R13" s="19">
+        <v>33</v>
+      </c>
+      <c r="S13" s="19">
+        <v>60</v>
+      </c>
+      <c r="T13" s="19">
+        <v>492</v>
+      </c>
+      <c r="U13" s="20">
+        <v>1097</v>
+      </c>
+      <c r="V13" s="20">
+        <v>1814</v>
+      </c>
+      <c r="W13" s="19">
+        <v>586</v>
+      </c>
+      <c r="X13" s="20">
+        <v>4098</v>
+      </c>
+      <c r="Y13" s="21">
+        <v>67641</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>5</v>
+      </c>
+      <c r="B14" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="33">
+        <v>52</v>
+      </c>
+      <c r="D14" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="38">
+        <v>16</v>
+      </c>
+      <c r="F14" s="38">
+        <v>33</v>
+      </c>
+      <c r="G14" s="38">
+        <v>60</v>
+      </c>
+      <c r="H14" s="38">
+        <v>492</v>
+      </c>
+      <c r="I14" s="41">
+        <v>1097</v>
+      </c>
+      <c r="J14" s="41">
+        <v>1814</v>
+      </c>
+      <c r="K14" s="38">
+        <v>586</v>
+      </c>
+      <c r="L14" s="40">
+        <v>67641</v>
+      </c>
+      <c r="P14" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q14" s="19">
+        <v>15</v>
+      </c>
+      <c r="R14" s="19">
+        <v>30</v>
+      </c>
+      <c r="S14" s="19">
+        <v>68</v>
+      </c>
+      <c r="T14" s="19">
+        <v>371</v>
+      </c>
+      <c r="U14" s="19">
+        <v>762</v>
+      </c>
+      <c r="V14" s="20">
+        <v>1201</v>
+      </c>
+      <c r="W14" s="20">
+        <v>1495</v>
+      </c>
+      <c r="X14" s="20">
+        <v>3942</v>
+      </c>
+      <c r="Y14" s="21">
+        <v>66534</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="33">
+        <v>57</v>
+      </c>
+      <c r="D15" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="38">
+        <v>15</v>
+      </c>
+      <c r="F15" s="38">
+        <v>30</v>
+      </c>
+      <c r="G15" s="38">
+        <v>68</v>
+      </c>
+      <c r="H15" s="38">
+        <v>371</v>
+      </c>
+      <c r="I15" s="38">
+        <v>762</v>
+      </c>
+      <c r="J15" s="41">
+        <v>1201</v>
+      </c>
+      <c r="K15" s="41">
+        <v>1495</v>
+      </c>
+      <c r="L15" s="40">
+        <v>66534</v>
+      </c>
+      <c r="P15" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q15" s="19">
+        <v>12</v>
+      </c>
+      <c r="R15" s="19">
+        <v>26</v>
+      </c>
+      <c r="S15" s="19">
+        <v>29</v>
+      </c>
+      <c r="T15" s="19">
+        <v>153</v>
+      </c>
+      <c r="U15" s="19">
+        <v>365</v>
+      </c>
+      <c r="V15" s="19">
+        <v>534</v>
+      </c>
+      <c r="W15" s="20">
+        <v>1099</v>
+      </c>
+      <c r="X15" s="20">
+        <v>2218</v>
+      </c>
+      <c r="Y15" s="21">
+        <v>69420</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="33">
+        <v>62</v>
+      </c>
+      <c r="D16" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="38">
+        <v>12</v>
+      </c>
+      <c r="F16" s="38">
+        <v>26</v>
+      </c>
+      <c r="G16" s="38">
+        <v>29</v>
+      </c>
+      <c r="H16" s="38">
+        <v>153</v>
+      </c>
+      <c r="I16" s="38">
+        <v>365</v>
+      </c>
+      <c r="J16" s="38">
+        <v>534</v>
+      </c>
+      <c r="K16" s="41">
+        <v>1099</v>
+      </c>
+      <c r="L16" s="40">
+        <v>69420</v>
+      </c>
+      <c r="P16" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q16" s="19">
+        <v>3</v>
+      </c>
+      <c r="R16" s="19">
+        <v>6</v>
+      </c>
+      <c r="S16" s="19">
+        <v>12</v>
+      </c>
+      <c r="T16" s="19">
+        <v>44</v>
+      </c>
+      <c r="U16" s="19">
+        <v>78</v>
+      </c>
+      <c r="V16" s="19">
+        <v>111</v>
+      </c>
+      <c r="W16" s="19">
+        <v>282</v>
+      </c>
+      <c r="X16" s="19">
+        <v>536</v>
+      </c>
+      <c r="Y16" s="21">
+        <v>72259</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>5</v>
+      </c>
+      <c r="B17" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="33">
+        <v>67</v>
+      </c>
+      <c r="D17" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="22">
-        <v>27</v>
-      </c>
-      <c r="E10" s="22">
+      <c r="E17" s="38">
+        <v>3</v>
+      </c>
+      <c r="F17" s="38">
+        <v>6</v>
+      </c>
+      <c r="G17" s="38">
+        <v>12</v>
+      </c>
+      <c r="H17" s="38">
+        <v>44</v>
+      </c>
+      <c r="I17" s="38">
+        <v>78</v>
+      </c>
+      <c r="J17" s="38">
+        <v>111</v>
+      </c>
+      <c r="K17" s="38">
+        <v>282</v>
+      </c>
+      <c r="L17" s="40">
+        <v>72259</v>
+      </c>
+      <c r="P17" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q17" s="23">
+        <v>3</v>
+      </c>
+      <c r="R17" s="23">
+        <v>4</v>
+      </c>
+      <c r="S17" s="23">
+        <v>1</v>
+      </c>
+      <c r="T17" s="23">
+        <v>8</v>
+      </c>
+      <c r="U17" s="23">
+        <v>13</v>
+      </c>
+      <c r="V17" s="23">
+        <v>20</v>
+      </c>
+      <c r="W17" s="23">
+        <v>108</v>
+      </c>
+      <c r="X17" s="23">
+        <v>157</v>
+      </c>
+      <c r="Y17" s="24">
+        <v>72048</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>5</v>
+      </c>
+      <c r="B18" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="33">
         <v>72</v>
       </c>
-      <c r="F10" s="22">
-        <v>12</v>
-      </c>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="22">
-        <v>140</v>
-      </c>
-      <c r="J10" s="23">
-        <v>8860211</v>
-      </c>
-      <c r="K10" s="24">
-        <v>63287</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="B11" s="22">
-        <v>26</v>
-      </c>
-      <c r="C11" s="22">
-        <v>40</v>
-      </c>
-      <c r="D11" s="22">
-        <v>70</v>
-      </c>
-      <c r="E11" s="22">
-        <v>640</v>
-      </c>
-      <c r="F11" s="22">
-        <v>336</v>
-      </c>
-      <c r="G11" s="22">
-        <v>34</v>
-      </c>
-      <c r="H11" s="20"/>
-      <c r="I11" s="23">
-        <v>1146</v>
-      </c>
-      <c r="J11" s="23">
-        <v>75190468</v>
-      </c>
-      <c r="K11" s="24">
-        <v>65611</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="B12" s="22">
+      <c r="D18" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="22">
-        <v>37</v>
-      </c>
-      <c r="D12" s="22">
-        <v>54</v>
-      </c>
-      <c r="E12" s="22">
-        <v>721</v>
-      </c>
-      <c r="F12" s="23">
-        <v>1066</v>
-      </c>
-      <c r="G12" s="22">
-        <v>774</v>
-      </c>
-      <c r="H12" s="22">
-        <v>73</v>
-      </c>
-      <c r="I12" s="23">
-        <v>2748</v>
-      </c>
-      <c r="J12" s="23">
-        <v>183447492</v>
-      </c>
-      <c r="K12" s="24">
-        <v>66757</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="B13" s="22">
-        <v>16</v>
-      </c>
-      <c r="C13" s="22">
-        <v>33</v>
-      </c>
-      <c r="D13" s="22">
-        <v>60</v>
-      </c>
-      <c r="E13" s="22">
-        <v>492</v>
-      </c>
-      <c r="F13" s="23">
-        <v>1097</v>
-      </c>
-      <c r="G13" s="23">
-        <v>1814</v>
-      </c>
-      <c r="H13" s="22">
-        <v>586</v>
-      </c>
-      <c r="I13" s="23">
-        <v>4098</v>
-      </c>
-      <c r="J13" s="23">
-        <v>277193635</v>
-      </c>
-      <c r="K13" s="24">
-        <v>67641</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="B14" s="22">
-        <v>15</v>
-      </c>
-      <c r="C14" s="22">
-        <v>30</v>
-      </c>
-      <c r="D14" s="22">
-        <v>68</v>
-      </c>
-      <c r="E14" s="22">
-        <v>371</v>
-      </c>
-      <c r="F14" s="22">
-        <v>762</v>
-      </c>
-      <c r="G14" s="23">
-        <v>1201</v>
-      </c>
-      <c r="H14" s="23">
-        <v>1495</v>
-      </c>
-      <c r="I14" s="23">
-        <v>3942</v>
-      </c>
-      <c r="J14" s="23">
-        <v>262278856</v>
-      </c>
-      <c r="K14" s="24">
-        <v>66534</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="B15" s="22">
-        <v>12</v>
-      </c>
-      <c r="C15" s="22">
-        <v>26</v>
-      </c>
-      <c r="D15" s="22">
-        <v>29</v>
-      </c>
-      <c r="E15" s="22">
-        <v>153</v>
-      </c>
-      <c r="F15" s="22">
-        <v>365</v>
-      </c>
-      <c r="G15" s="22">
-        <v>534</v>
-      </c>
-      <c r="H15" s="23">
-        <v>1099</v>
-      </c>
-      <c r="I15" s="23">
-        <v>2218</v>
-      </c>
-      <c r="J15" s="23">
-        <v>153973659</v>
-      </c>
-      <c r="K15" s="24">
-        <v>69420</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="B16" s="22">
+      <c r="E18" s="38">
         <v>3</v>
       </c>
-      <c r="C16" s="22">
-        <v>6</v>
-      </c>
-      <c r="D16" s="22">
-        <v>12</v>
-      </c>
-      <c r="E16" s="22">
-        <v>44</v>
-      </c>
-      <c r="F16" s="22">
-        <v>78</v>
-      </c>
-      <c r="G16" s="22">
-        <v>111</v>
-      </c>
-      <c r="H16" s="22">
-        <v>282</v>
-      </c>
-      <c r="I16" s="22">
-        <v>536</v>
-      </c>
-      <c r="J16" s="23">
-        <v>38731048</v>
-      </c>
-      <c r="K16" s="24">
-        <v>72259</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="25" t="s">
+      <c r="F18" s="38">
+        <v>4</v>
+      </c>
+      <c r="G18" s="38">
+        <v>1</v>
+      </c>
+      <c r="H18" s="38">
+        <v>8</v>
+      </c>
+      <c r="I18" s="38">
+        <v>13</v>
+      </c>
+      <c r="J18" s="38">
+        <v>20</v>
+      </c>
+      <c r="K18" s="38">
+        <v>108</v>
+      </c>
+      <c r="L18" s="40">
+        <v>72048</v>
+      </c>
+      <c r="P18" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="B17" s="26">
-        <v>3</v>
-      </c>
-      <c r="C17" s="26">
-        <v>4</v>
-      </c>
-      <c r="D17" s="26">
-        <v>1</v>
-      </c>
-      <c r="E17" s="26">
-        <v>8</v>
-      </c>
-      <c r="F17" s="26">
-        <v>13</v>
-      </c>
-      <c r="G17" s="26">
-        <v>20</v>
-      </c>
-      <c r="H17" s="26">
-        <v>108</v>
-      </c>
-      <c r="I17" s="26">
-        <v>157</v>
-      </c>
-      <c r="J17" s="27">
-        <v>11311583</v>
-      </c>
-      <c r="K17" s="28">
-        <v>72048</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="29" t="s">
-        <v>96</v>
-      </c>
-      <c r="B18" s="30">
+      <c r="Q18" s="26">
         <v>105</v>
       </c>
-      <c r="C18" s="30">
+      <c r="R18" s="26">
         <v>198</v>
       </c>
-      <c r="D18" s="30">
+      <c r="S18" s="26">
         <v>321</v>
       </c>
-      <c r="E18" s="31">
+      <c r="T18" s="27">
         <v>2501</v>
       </c>
-      <c r="F18" s="31">
+      <c r="U18" s="27">
         <v>3729</v>
       </c>
-      <c r="G18" s="31">
+      <c r="V18" s="27">
         <v>4488</v>
       </c>
-      <c r="H18" s="31">
+      <c r="W18" s="27">
         <v>3643</v>
       </c>
-      <c r="I18" s="31">
+      <c r="X18" s="27">
         <v>14985</v>
       </c>
-      <c r="J18" s="32">
-        <v>1010986952</v>
-      </c>
-      <c r="K18" s="33">
+      <c r="Y18" s="28">
         <v>67467</v>
       </c>
     </row>
+    <row r="19" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="L19" s="35"/>
+    </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:H6"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="J6:J7"/>
-    <mergeCell ref="K6:K7"/>
+  <mergeCells count="4">
+    <mergeCell ref="P6:P7"/>
+    <mergeCell ref="Q6:W6"/>
+    <mergeCell ref="X6:X7"/>
+    <mergeCell ref="Y6:Y7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="TOC!A1" display="TOC"/>
@@ -2425,7 +3148,7 @@
   <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+      <selection activeCell="A5" sqref="A5:K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2567,13 +3290,13 @@
       <c r="D7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="35"/>
-      <c r="I7" s="35"/>
-      <c r="J7" s="35"/>
-      <c r="K7" s="35"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="30"/>
+      <c r="K7" s="30"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
@@ -2585,13 +3308,13 @@
       <c r="D8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="35"/>
-      <c r="J8" s="35"/>
-      <c r="K8" s="35"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="30"/>
+      <c r="J8" s="30"/>
+      <c r="K8" s="30"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -2606,13 +3329,13 @@
       <c r="D9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="35"/>
-      <c r="J9" s="35"/>
-      <c r="K9" s="35"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="30"/>
+      <c r="K9" s="30"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
@@ -2624,13 +3347,13 @@
       <c r="D10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="35"/>
-      <c r="J10" s="35"/>
-      <c r="K10" s="35"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="30"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -2645,15 +3368,15 @@
       <c r="D11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35">
-        <v>5</v>
-      </c>
-      <c r="G11" s="35"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="35"/>
-      <c r="J11" s="35"/>
-      <c r="K11" s="35"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30">
+        <v>5</v>
+      </c>
+      <c r="G11" s="30"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="30"/>
+      <c r="K11" s="30"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
@@ -2665,15 +3388,15 @@
       <c r="D12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35">
+      <c r="E12" s="30"/>
+      <c r="F12" s="30">
         <v>51550.8</v>
       </c>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="35"/>
-      <c r="K12" s="35"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="30"/>
+      <c r="K12" s="30"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -2688,23 +3411,23 @@
       <c r="D13" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="35">
+      <c r="E13" s="30">
         <v>20</v>
       </c>
-      <c r="F13" s="35">
+      <c r="F13" s="30">
         <v>27</v>
       </c>
-      <c r="G13" s="35">
+      <c r="G13" s="30">
         <v>49</v>
       </c>
-      <c r="H13" s="35">
+      <c r="H13" s="30">
         <v>131</v>
       </c>
-      <c r="I13" s="35">
+      <c r="I13" s="30">
         <v>26</v>
       </c>
-      <c r="J13" s="35"/>
-      <c r="K13" s="35"/>
+      <c r="J13" s="30"/>
+      <c r="K13" s="30"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
@@ -2716,23 +3439,23 @@
       <c r="D14" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="35">
+      <c r="E14" s="30">
         <v>62901.596849999994</v>
       </c>
-      <c r="F14" s="35">
+      <c r="F14" s="30">
         <v>62901.596851851849</v>
       </c>
-      <c r="G14" s="35">
+      <c r="G14" s="30">
         <v>62901.596836734694</v>
       </c>
-      <c r="H14" s="35">
+      <c r="H14" s="30">
         <v>62901.596839694656</v>
       </c>
-      <c r="I14" s="35">
+      <c r="I14" s="30">
         <v>62901.596846153843</v>
       </c>
-      <c r="J14" s="35"/>
-      <c r="K14" s="35"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="30"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -2747,25 +3470,25 @@
       <c r="D15" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="35">
+      <c r="E15" s="30">
         <v>40</v>
       </c>
-      <c r="F15" s="35">
+      <c r="F15" s="30">
         <v>41</v>
       </c>
-      <c r="G15" s="35">
+      <c r="G15" s="30">
         <v>94</v>
       </c>
-      <c r="H15" s="35">
+      <c r="H15" s="30">
         <v>904</v>
       </c>
-      <c r="I15" s="35">
+      <c r="I15" s="30">
         <v>398</v>
       </c>
-      <c r="J15" s="35">
+      <c r="J15" s="30">
         <v>36</v>
       </c>
-      <c r="K15" s="35"/>
+      <c r="K15" s="30"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
@@ -2777,25 +3500,25 @@
       <c r="D16" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="35">
+      <c r="E16" s="30">
         <v>64650.206874999996</v>
       </c>
-      <c r="F16" s="35">
+      <c r="F16" s="30">
         <v>64650.206878048775</v>
       </c>
-      <c r="G16" s="35">
+      <c r="G16" s="30">
         <v>64650.20687234043</v>
       </c>
-      <c r="H16" s="35">
+      <c r="H16" s="30">
         <v>64650.206869469024</v>
       </c>
-      <c r="I16" s="35">
+      <c r="I16" s="30">
         <v>64650.206884422107</v>
       </c>
-      <c r="J16" s="35">
+      <c r="J16" s="30">
         <v>64650.206861111117</v>
       </c>
-      <c r="K16" s="35"/>
+      <c r="K16" s="30"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
@@ -2810,25 +3533,25 @@
       <c r="D17" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E17" s="35">
+      <c r="E17" s="30">
         <v>38</v>
       </c>
-      <c r="F17" s="35">
+      <c r="F17" s="30">
         <v>35</v>
       </c>
-      <c r="G17" s="35">
+      <c r="G17" s="30">
         <v>85</v>
       </c>
-      <c r="H17" s="35">
+      <c r="H17" s="30">
         <v>855</v>
       </c>
-      <c r="I17" s="35">
+      <c r="I17" s="30">
         <v>1283</v>
       </c>
-      <c r="J17" s="35">
+      <c r="J17" s="30">
         <v>787</v>
       </c>
-      <c r="K17" s="35">
+      <c r="K17" s="30">
         <v>67</v>
       </c>
     </row>
@@ -2842,25 +3565,25 @@
       <c r="D18" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E18" s="35">
+      <c r="E18" s="30">
         <v>65749.671105263158</v>
       </c>
-      <c r="F18" s="35">
+      <c r="F18" s="30">
         <v>65749.671114285709</v>
       </c>
-      <c r="G18" s="35">
+      <c r="G18" s="30">
         <v>65749.671105882357</v>
       </c>
-      <c r="H18" s="35">
+      <c r="H18" s="30">
         <v>65749.671111111107</v>
       </c>
-      <c r="I18" s="35">
+      <c r="I18" s="30">
         <v>65749.67111457522</v>
       </c>
-      <c r="J18" s="35">
+      <c r="J18" s="30">
         <v>65749.671105463785</v>
       </c>
-      <c r="K18" s="35">
+      <c r="K18" s="30">
         <v>65749.671104477602</v>
       </c>
     </row>
@@ -2877,25 +3600,25 @@
       <c r="D19" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E19" s="35">
+      <c r="E19" s="30">
         <v>31</v>
       </c>
-      <c r="F19" s="35">
+      <c r="F19" s="30">
         <v>30</v>
       </c>
-      <c r="G19" s="35">
+      <c r="G19" s="30">
         <v>81</v>
       </c>
-      <c r="H19" s="35">
+      <c r="H19" s="30">
         <v>640</v>
       </c>
-      <c r="I19" s="35">
+      <c r="I19" s="30">
         <v>1386</v>
       </c>
-      <c r="J19" s="35">
+      <c r="J19" s="30">
         <v>1724</v>
       </c>
-      <c r="K19" s="35">
+      <c r="K19" s="30">
         <v>594</v>
       </c>
     </row>
@@ -2909,25 +3632,25 @@
       <c r="D20" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E20" s="35">
+      <c r="E20" s="30">
         <v>65309.034548387099</v>
       </c>
-      <c r="F20" s="35">
+      <c r="F20" s="30">
         <v>65309.034566666669</v>
       </c>
-      <c r="G20" s="35">
+      <c r="G20" s="30">
         <v>65309.034555555554</v>
       </c>
-      <c r="H20" s="35">
+      <c r="H20" s="30">
         <v>65309.034546875002</v>
       </c>
-      <c r="I20" s="35">
+      <c r="I20" s="30">
         <v>65309.034552669553</v>
       </c>
-      <c r="J20" s="35">
+      <c r="J20" s="30">
         <v>65309.03457076566</v>
       </c>
-      <c r="K20" s="35">
+      <c r="K20" s="30">
         <v>65309.034545454553</v>
       </c>
     </row>
@@ -2944,25 +3667,25 @@
       <c r="D21" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E21" s="35">
+      <c r="E21" s="30">
         <v>24</v>
       </c>
-      <c r="F21" s="35">
+      <c r="F21" s="30">
         <v>34</v>
       </c>
-      <c r="G21" s="35">
+      <c r="G21" s="30">
         <v>67</v>
       </c>
-      <c r="H21" s="35">
+      <c r="H21" s="30">
         <v>489</v>
       </c>
-      <c r="I21" s="35">
+      <c r="I21" s="30">
         <v>913</v>
       </c>
-      <c r="J21" s="35">
+      <c r="J21" s="30">
         <v>1115</v>
       </c>
-      <c r="K21" s="35">
+      <c r="K21" s="30">
         <v>1584</v>
       </c>
     </row>
@@ -2976,25 +3699,25 @@
       <c r="D22" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E22" s="35">
+      <c r="E22" s="30">
         <v>64977.174874999997</v>
       </c>
-      <c r="F22" s="35">
+      <c r="F22" s="30">
         <v>64977.174882352941</v>
       </c>
-      <c r="G22" s="35">
+      <c r="G22" s="30">
         <v>64977.174865671645</v>
       </c>
-      <c r="H22" s="35">
+      <c r="H22" s="30">
         <v>64977.174867075672</v>
       </c>
-      <c r="I22" s="35">
+      <c r="I22" s="30">
         <v>64977.174874041615</v>
       </c>
-      <c r="J22" s="35">
+      <c r="J22" s="30">
         <v>64977.174869955161</v>
       </c>
-      <c r="K22" s="35">
+      <c r="K22" s="30">
         <v>64977.174873737371</v>
       </c>
     </row>
@@ -3011,25 +3734,25 @@
       <c r="D23" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E23" s="35">
+      <c r="E23" s="30">
         <v>10</v>
       </c>
-      <c r="F23" s="35">
+      <c r="F23" s="30">
         <v>25</v>
       </c>
-      <c r="G23" s="35">
+      <c r="G23" s="30">
         <v>30</v>
       </c>
-      <c r="H23" s="35">
+      <c r="H23" s="30">
         <v>222</v>
       </c>
-      <c r="I23" s="35">
+      <c r="I23" s="30">
         <v>443</v>
       </c>
-      <c r="J23" s="35">
+      <c r="J23" s="30">
         <v>481</v>
       </c>
-      <c r="K23" s="35">
+      <c r="K23" s="30">
         <v>1003</v>
       </c>
     </row>
@@ -3043,25 +3766,25 @@
       <c r="D24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E24" s="35">
+      <c r="E24" s="30">
         <v>67083.991420000006</v>
       </c>
-      <c r="F24" s="35">
+      <c r="F24" s="30">
         <v>67083.991399999999</v>
       </c>
-      <c r="G24" s="35">
+      <c r="G24" s="30">
         <v>67083.991433333329</v>
       </c>
-      <c r="H24" s="35">
+      <c r="H24" s="30">
         <v>67083.991396396392</v>
       </c>
-      <c r="I24" s="35">
+      <c r="I24" s="30">
         <v>67083.991422121893</v>
       </c>
-      <c r="J24" s="35">
+      <c r="J24" s="30">
         <v>67083.991413721422</v>
       </c>
-      <c r="K24" s="35">
+      <c r="K24" s="30">
         <v>67083.991415752738</v>
       </c>
     </row>
@@ -3078,25 +3801,25 @@
       <c r="D25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E25" s="35">
+      <c r="E25" s="30">
         <v>4</v>
       </c>
-      <c r="F25" s="35">
+      <c r="F25" s="30">
         <v>7</v>
       </c>
-      <c r="G25" s="35">
+      <c r="G25" s="30">
         <v>14</v>
       </c>
-      <c r="H25" s="35">
+      <c r="H25" s="30">
         <v>50</v>
       </c>
-      <c r="I25" s="35">
+      <c r="I25" s="30">
         <v>80</v>
       </c>
-      <c r="J25" s="35">
+      <c r="J25" s="30">
         <v>90</v>
       </c>
-      <c r="K25" s="35">
+      <c r="K25" s="30">
         <v>225</v>
       </c>
     </row>
@@ -3110,25 +3833,25 @@
       <c r="D26" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E26" s="35">
+      <c r="E26" s="30">
         <v>71981.521275000006</v>
       </c>
-      <c r="F26" s="35">
+      <c r="F26" s="30">
         <v>71981.521271428574</v>
       </c>
-      <c r="G26" s="35">
+      <c r="G26" s="30">
         <v>71981.521285714276</v>
       </c>
-      <c r="H26" s="35">
+      <c r="H26" s="30">
         <v>71981.521280000001</v>
       </c>
-      <c r="I26" s="35">
+      <c r="I26" s="30">
         <v>71981.521274999992</v>
       </c>
-      <c r="J26" s="35">
+      <c r="J26" s="30">
         <v>71981.521277777778</v>
       </c>
-      <c r="K26" s="35">
+      <c r="K26" s="30">
         <v>71981.521288888878</v>
       </c>
     </row>
@@ -3145,25 +3868,25 @@
       <c r="D27" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E27" s="35">
+      <c r="E27" s="30">
         <v>3</v>
       </c>
-      <c r="F27" s="35">
+      <c r="F27" s="30">
         <v>1</v>
       </c>
-      <c r="G27" s="35">
+      <c r="G27" s="30">
         <v>1</v>
       </c>
-      <c r="H27" s="35">
-        <v>5</v>
-      </c>
-      <c r="I27" s="35">
+      <c r="H27" s="30">
+        <v>5</v>
+      </c>
+      <c r="I27" s="30">
         <v>23</v>
       </c>
-      <c r="J27" s="35">
+      <c r="J27" s="30">
         <v>14</v>
       </c>
-      <c r="K27" s="35">
+      <c r="K27" s="30">
         <v>102</v>
       </c>
     </row>
@@ -3174,25 +3897,25 @@
       <c r="D28" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E28" s="35">
+      <c r="E28" s="30">
         <v>71843.617433333333</v>
       </c>
-      <c r="F28" s="35">
+      <c r="F28" s="30">
         <v>71843.617450000005</v>
       </c>
-      <c r="G28" s="35">
+      <c r="G28" s="30">
         <v>71843.617450000005</v>
       </c>
-      <c r="H28" s="35">
+      <c r="H28" s="30">
         <v>71843.617440000002</v>
       </c>
-      <c r="I28" s="35">
+      <c r="I28" s="30">
         <v>71843.617434782602</v>
       </c>
-      <c r="J28" s="35">
+      <c r="J28" s="30">
         <v>71843.617428571422</v>
       </c>
-      <c r="K28" s="35">
+      <c r="K28" s="30">
         <v>71843.617450980397</v>
       </c>
     </row>
@@ -3210,7 +3933,7 @@
   <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3938,21 +4661,20 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P17"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="9.140625" customWidth="1"/>
-    <col min="12" max="12" width="18.28515625" customWidth="1"/>
-    <col min="13" max="15" width="14.5703125" customWidth="1"/>
-    <col min="16" max="16" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.28515625" customWidth="1"/>
+    <col min="11" max="13" width="14.5703125" customWidth="1"/>
+    <col min="14" max="14" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3965,17 +4687,13 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="P1" s="1"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N1" s="1"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>98</v>
-      </c>
+      <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -3984,17 +4702,13 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="P2" s="2"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N2" s="2"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>99</v>
-      </c>
+      <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -4003,292 +4717,13 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="P3" s="2"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>25</v>
-      </c>
-      <c r="B5" t="s">
-        <v>97</v>
-      </c>
-      <c r="C5" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="34" t="s">
-        <v>70</v>
-      </c>
-      <c r="E5" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="34">
-        <v>27</v>
-      </c>
-      <c r="D6" s="34">
-        <v>533</v>
-      </c>
-      <c r="E6" s="34">
-        <f>F6/D6</f>
-        <v>1615.7913193245779</v>
-      </c>
-      <c r="F6">
-        <v>861216.77320000005</v>
-      </c>
-      <c r="G6">
-        <f>E6*12</f>
-        <v>19389.495831894936</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="34">
-        <v>32</v>
-      </c>
-      <c r="D7" s="34">
-        <v>1010</v>
-      </c>
-      <c r="E7" s="34">
-        <f t="shared" ref="E7:E17" si="0">F7/D7</f>
-        <v>1615.7913198019803</v>
-      </c>
-      <c r="F7">
-        <v>1631949.233</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>5</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="34">
-        <v>37</v>
-      </c>
-      <c r="D8" s="34">
-        <v>3503</v>
-      </c>
-      <c r="E8" s="34">
-        <f t="shared" si="0"/>
-        <v>1615.7913194404796</v>
-      </c>
-      <c r="F8">
-        <v>5660116.9919999996</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>5</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="34">
-        <v>42</v>
-      </c>
-      <c r="D9" s="34">
-        <v>7419</v>
-      </c>
-      <c r="E9" s="34">
-        <f t="shared" si="0"/>
-        <v>1615.7913195848498</v>
-      </c>
-      <c r="F9">
-        <v>11987555.800000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>5</v>
-      </c>
-      <c r="B10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="34">
-        <v>47</v>
-      </c>
-      <c r="D10" s="34">
-        <v>6631</v>
-      </c>
-      <c r="E10" s="34">
-        <f t="shared" si="0"/>
-        <v>1615.7913195596441</v>
-      </c>
-      <c r="F10">
-        <v>10714312.24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>5</v>
-      </c>
-      <c r="B11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="34">
-        <v>52</v>
-      </c>
-      <c r="D11" s="34">
-        <v>4813</v>
-      </c>
-      <c r="E11" s="34">
-        <f t="shared" si="0"/>
-        <v>1615.7913193434449</v>
-      </c>
-      <c r="F11">
-        <v>7776803.6200000001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>5</v>
-      </c>
-      <c r="B12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="34">
-        <v>57</v>
-      </c>
-      <c r="D12" s="34">
-        <v>3457</v>
-      </c>
-      <c r="E12" s="34">
-        <f t="shared" si="0"/>
-        <v>1615.7913193520394</v>
-      </c>
-      <c r="F12">
-        <v>5585790.591</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>5</v>
-      </c>
-      <c r="B13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="34">
-        <v>62</v>
-      </c>
-      <c r="D13" s="34">
-        <v>2455</v>
-      </c>
-      <c r="E13" s="34">
-        <f t="shared" si="0"/>
-        <v>1615.7913193482686</v>
-      </c>
-      <c r="F13">
-        <v>3966767.6889999998</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>5</v>
-      </c>
-      <c r="B14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="34">
-        <v>67</v>
-      </c>
-      <c r="D14" s="34">
-        <v>1626</v>
-      </c>
-      <c r="E14" s="34">
-        <f t="shared" si="0"/>
-        <v>1615.7913191881919</v>
-      </c>
-      <c r="F14">
-        <v>2627276.6850000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>5</v>
-      </c>
-      <c r="B15" t="s">
-        <v>67</v>
-      </c>
-      <c r="C15" s="34">
-        <v>72</v>
-      </c>
-      <c r="D15" s="34">
-        <v>731</v>
-      </c>
-      <c r="E15" s="34">
-        <f t="shared" si="0"/>
-        <v>1615.7913187414499</v>
-      </c>
-      <c r="F15">
-        <v>1181143.4539999999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>5</v>
-      </c>
-      <c r="B16" t="s">
-        <v>68</v>
-      </c>
-      <c r="C16" s="34">
-        <v>77</v>
-      </c>
-      <c r="D16" s="34">
-        <v>201</v>
-      </c>
-      <c r="E16" s="34">
-        <f t="shared" si="0"/>
-        <v>1615.791319402985</v>
-      </c>
-      <c r="F16">
-        <v>324774.0552</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>5</v>
-      </c>
-      <c r="B17" t="s">
-        <v>69</v>
-      </c>
-      <c r="C17" s="34">
-        <v>82</v>
-      </c>
-      <c r="D17" s="34">
-        <v>15</v>
-      </c>
-      <c r="E17" s="34">
-        <f t="shared" si="0"/>
-        <v>1615.7913193333334</v>
-      </c>
-      <c r="F17">
-        <v>24236.869790000001</v>
-      </c>
+      <c r="N3" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" location="TOC!A1" display="TOC"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update scripts for loading member data
</commit_message>
<xml_diff>
--- a/Data_inputs/MISERS_MemberData.xlsx
+++ b/Data_inputs/MISERS_MemberData.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="111">
   <si>
     <t>TOC</t>
   </si>
@@ -518,34 +518,49 @@
     </r>
   </si>
   <si>
-    <t>age.grp</t>
-  </si>
-  <si>
-    <t>C5</t>
-  </si>
-  <si>
-    <t>E17</t>
-  </si>
-  <si>
     <t>conservation</t>
   </si>
   <si>
     <t>correction</t>
   </si>
   <si>
-    <t>other</t>
-  </si>
-  <si>
     <t>salary.avg</t>
   </si>
   <si>
-    <t>L18</t>
-  </si>
-  <si>
     <t>male</t>
   </si>
   <si>
     <t>female</t>
+  </si>
+  <si>
+    <t>K29</t>
+  </si>
+  <si>
+    <t>benperiod</t>
+  </si>
+  <si>
+    <t>month</t>
+  </si>
+  <si>
+    <t>name_N</t>
+  </si>
+  <si>
+    <t>name_V</t>
+  </si>
+  <si>
+    <t>benefit</t>
+  </si>
+  <si>
+    <t>E20</t>
+  </si>
+  <si>
+    <t>nretirees</t>
+  </si>
+  <si>
+    <t>B8</t>
+  </si>
+  <si>
+    <t>others</t>
   </si>
 </sst>
 </file>
@@ -555,7 +570,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0;&quot;$&quot;\-#,##0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -603,6 +618,30 @@
     <font>
       <sz val="12"/>
       <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -716,7 +755,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -806,26 +845,46 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="3"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="3"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" indent="3"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="9" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="11" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="11" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="10" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -851,13 +910,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>933450</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>8420</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>503720</xdr:colOff>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>189836</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1066,13 +1125,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>437976</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>94912</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1104,13 +1163,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>666750</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>76031</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>152055</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1142,13 +1201,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>914400</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1729,10 +1788,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P17"/>
+  <dimension ref="A1:P20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1765,7 +1824,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -1784,7 +1843,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -1798,279 +1857,336 @@
       <c r="L3" s="2"/>
       <c r="P3" s="2"/>
     </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="P4" s="2"/>
+    </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>25</v>
-      </c>
-      <c r="B5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C5" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="29" t="s">
-        <v>70</v>
-      </c>
-      <c r="E5" s="29" t="s">
-        <v>71</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
+      <c r="A5" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="P5" s="2"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="29">
-        <v>27</v>
-      </c>
-      <c r="D6" s="29">
-        <v>533</v>
-      </c>
-      <c r="E6" s="29">
-        <f>F6/D6</f>
-        <v>1615.7913193245779</v>
-      </c>
-      <c r="F6">
-        <v>861216.77320000005</v>
-      </c>
-      <c r="G6">
-        <f>E6*12</f>
-        <v>19389.495831894936</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="29">
-        <v>32</v>
-      </c>
-      <c r="D7" s="29">
-        <v>1010</v>
-      </c>
-      <c r="E7" s="29">
-        <f t="shared" ref="E7:E17" si="0">F7/D7</f>
-        <v>1615.7913198019803</v>
-      </c>
-      <c r="F7">
-        <v>1631949.233</v>
-      </c>
+      <c r="A6" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="P6" s="2"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="29">
+        <v>27</v>
+      </c>
+      <c r="D9" s="29">
+        <v>533</v>
+      </c>
+      <c r="E9" s="29">
+        <f>F9/D9</f>
+        <v>1615.7913193245779</v>
+      </c>
+      <c r="F9">
+        <v>861216.77320000005</v>
+      </c>
+      <c r="G9">
+        <f>E9*12</f>
+        <v>19389.495831894936</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="29">
+        <v>32</v>
+      </c>
+      <c r="D10" s="29">
+        <v>1010</v>
+      </c>
+      <c r="E10" s="29">
+        <f t="shared" ref="E10:E20" si="0">F10/D10</f>
+        <v>1615.7913198019803</v>
+      </c>
+      <c r="F10">
+        <v>1631949.233</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="29">
+      <c r="C11" s="29">
         <v>37</v>
       </c>
-      <c r="D8" s="29">
+      <c r="D11" s="29">
         <v>3503</v>
       </c>
-      <c r="E8" s="29">
+      <c r="E11" s="29">
         <f t="shared" si="0"/>
         <v>1615.7913194404796</v>
       </c>
-      <c r="F8">
+      <c r="F11">
         <v>5660116.9919999996</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>5</v>
-      </c>
-      <c r="B9" t="s">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="29">
+      <c r="C12" s="29">
         <v>42</v>
       </c>
-      <c r="D9" s="29">
+      <c r="D12" s="29">
         <v>7419</v>
       </c>
-      <c r="E9" s="29">
+      <c r="E12" s="29">
         <f t="shared" si="0"/>
         <v>1615.7913195848498</v>
       </c>
-      <c r="F9">
+      <c r="F12">
         <v>11987555.800000001</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>5</v>
-      </c>
-      <c r="B10" t="s">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="29">
+      <c r="C13" s="29">
         <v>47</v>
       </c>
-      <c r="D10" s="29">
+      <c r="D13" s="29">
         <v>6631</v>
       </c>
-      <c r="E10" s="29">
+      <c r="E13" s="29">
         <f t="shared" si="0"/>
         <v>1615.7913195596441</v>
       </c>
-      <c r="F10">
+      <c r="F13">
         <v>10714312.24</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>5</v>
-      </c>
-      <c r="B11" t="s">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="29">
+      <c r="C14" s="29">
         <v>52</v>
       </c>
-      <c r="D11" s="29">
+      <c r="D14" s="29">
         <v>4813</v>
       </c>
-      <c r="E11" s="29">
+      <c r="E14" s="29">
         <f t="shared" si="0"/>
         <v>1615.7913193434449</v>
       </c>
-      <c r="F11">
+      <c r="F14">
         <v>7776803.6200000001</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>5</v>
-      </c>
-      <c r="B12" t="s">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="29">
+      <c r="C15" s="29">
         <v>57</v>
       </c>
-      <c r="D12" s="29">
+      <c r="D15" s="29">
         <v>3457</v>
       </c>
-      <c r="E12" s="29">
+      <c r="E15" s="29">
         <f t="shared" si="0"/>
         <v>1615.7913193520394</v>
       </c>
-      <c r="F12">
+      <c r="F15">
         <v>5585790.591</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>5</v>
-      </c>
-      <c r="B13" t="s">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="29">
+      <c r="C16" s="29">
         <v>62</v>
       </c>
-      <c r="D13" s="29">
+      <c r="D16" s="29">
         <v>2455</v>
       </c>
-      <c r="E13" s="29">
+      <c r="E16" s="29">
         <f t="shared" si="0"/>
         <v>1615.7913193482686</v>
       </c>
-      <c r="F13">
+      <c r="F16">
         <v>3966767.6889999998</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>5</v>
-      </c>
-      <c r="B14" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>5</v>
+      </c>
+      <c r="B17" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="29">
+      <c r="C17" s="29">
         <v>67</v>
       </c>
-      <c r="D14" s="29">
+      <c r="D17" s="29">
         <v>1626</v>
       </c>
-      <c r="E14" s="29">
+      <c r="E17" s="29">
         <f t="shared" si="0"/>
         <v>1615.7913191881919</v>
       </c>
-      <c r="F14">
+      <c r="F17">
         <v>2627276.6850000001</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>5</v>
-      </c>
-      <c r="B15" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
         <v>67</v>
       </c>
-      <c r="C15" s="29">
+      <c r="C18" s="29">
         <v>72</v>
       </c>
-      <c r="D15" s="29">
+      <c r="D18" s="29">
         <v>731</v>
       </c>
-      <c r="E15" s="29">
+      <c r="E18" s="29">
         <f t="shared" si="0"/>
         <v>1615.7913187414499</v>
       </c>
-      <c r="F15">
+      <c r="F18">
         <v>1181143.4539999999</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>5</v>
-      </c>
-      <c r="B16" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>5</v>
+      </c>
+      <c r="B19" t="s">
         <v>68</v>
       </c>
-      <c r="C16" s="29">
+      <c r="C19" s="29">
         <v>77</v>
       </c>
-      <c r="D16" s="29">
+      <c r="D19" s="29">
         <v>201</v>
       </c>
-      <c r="E16" s="29">
+      <c r="E19" s="29">
         <f t="shared" si="0"/>
         <v>1615.791319402985</v>
       </c>
-      <c r="F16">
+      <c r="F19">
         <v>324774.0552</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>5</v>
-      </c>
-      <c r="B17" t="s">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>5</v>
+      </c>
+      <c r="B20" t="s">
         <v>69</v>
       </c>
-      <c r="C17" s="29">
+      <c r="C20" s="29">
         <v>82</v>
       </c>
-      <c r="D17" s="29">
+      <c r="D20" s="29">
         <v>15</v>
       </c>
-      <c r="E17" s="29">
+      <c r="E20" s="29">
         <f t="shared" si="0"/>
         <v>1615.7913193333334</v>
       </c>
-      <c r="F17">
+      <c r="F20">
         <v>24236.869790000001</v>
       </c>
     </row>
@@ -2089,7 +2205,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2124,13 +2240,13 @@
         <v>61</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="F6" s="9" t="s">
         <v>64</v>
@@ -2237,10 +2353,10 @@
         <v>61</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2289,15 +2405,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y19"/>
+  <dimension ref="A1:Y29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="10" max="12" width="14.5703125" customWidth="1"/>
+    <col min="5" max="12" width="15.42578125" style="42" customWidth="1"/>
     <col min="13" max="13" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="16.28515625" customWidth="1"/>
     <col min="25" max="25" width="13.42578125" customWidth="1"/>
@@ -2310,11 +2426,11 @@
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
       <c r="M1" s="1"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
@@ -2326,11 +2442,11 @@
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
       <c r="M2" s="2"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -2338,50 +2454,50 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
       <c r="M3" s="2"/>
     </row>
     <row r="6" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="42" t="s">
+      <c r="C6" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="42" t="s">
+      <c r="D6" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="43">
+      <c r="E6" s="44">
         <v>2</v>
       </c>
-      <c r="F6" s="43">
+      <c r="F6" s="44">
         <v>7</v>
       </c>
-      <c r="G6" s="43">
+      <c r="G6" s="44">
         <v>12</v>
       </c>
-      <c r="H6" s="43">
+      <c r="H6" s="44">
         <v>17</v>
       </c>
-      <c r="I6" s="43">
+      <c r="I6" s="44">
         <v>22</v>
       </c>
-      <c r="J6" s="43">
+      <c r="J6" s="44">
         <v>27</v>
       </c>
-      <c r="K6" s="43">
+      <c r="K6" s="44">
         <v>32</v>
       </c>
-      <c r="L6" s="42" t="s">
-        <v>102</v>
+      <c r="L6" s="45" t="s">
+        <v>98</v>
       </c>
       <c r="P6" s="31" t="s">
         <v>72</v>
@@ -2403,33 +2519,33 @@
       </c>
     </row>
     <row r="7" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="33" t="s">
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="33" t="s">
+      <c r="F7" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="33" t="s">
-        <v>5</v>
-      </c>
-      <c r="H7" s="33" t="s">
+      <c r="G7" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="H7" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="I7" s="33" t="s">
+      <c r="I7" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="J7" s="33" t="s">
+      <c r="J7" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="K7" s="33" t="s">
+      <c r="K7" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="L7" s="36"/>
+      <c r="L7" s="47"/>
       <c r="P7" s="31"/>
       <c r="Q7" s="10" t="s">
         <v>76</v>
@@ -2455,11 +2571,11 @@
       <c r="X7" s="32"/>
       <c r="Y7" s="32"/>
     </row>
-    <row r="8" spans="1:25" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="37" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="33">
@@ -2468,14 +2584,14 @@
       <c r="D8" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37"/>
-      <c r="J8" s="37"/>
-      <c r="K8" s="37"/>
-      <c r="L8" s="36"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="50"/>
+      <c r="G8" s="50"/>
+      <c r="H8" s="50"/>
+      <c r="I8" s="50"/>
+      <c r="J8" s="50"/>
+      <c r="K8" s="50"/>
+      <c r="L8" s="51"/>
       <c r="P8" s="11" t="s">
         <v>83</v>
       </c>
@@ -2495,638 +2611,1052 @@
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>5</v>
-      </c>
-      <c r="B9" s="36" t="s">
-        <v>14</v>
+    <row r="9" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="37" t="s">
+        <v>16</v>
       </c>
       <c r="C9" s="33">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D9" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="37"/>
-      <c r="I9" s="37"/>
-      <c r="J9" s="37"/>
-      <c r="K9" s="37"/>
-      <c r="L9" s="36"/>
-      <c r="P9" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="Q9" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="R9" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="S9" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="T9" s="16" t="s">
-        <v>84</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="E9" s="50"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="50"/>
+      <c r="I9" s="50"/>
+      <c r="J9" s="50"/>
+      <c r="K9" s="50"/>
+      <c r="L9" s="51"/>
+      <c r="P9" s="38"/>
+      <c r="Q9" s="39"/>
+      <c r="R9" s="17"/>
+      <c r="S9" s="17"/>
+      <c r="T9" s="17"/>
       <c r="U9" s="17"/>
       <c r="V9" s="17"/>
       <c r="W9" s="17"/>
-      <c r="X9" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="Y9" s="18" t="s">
-        <v>84</v>
-      </c>
+      <c r="X9" s="39"/>
+      <c r="Y9" s="40"/>
     </row>
     <row r="10" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>5</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="35" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="33">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D10" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="37"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="37"/>
-      <c r="H10" s="37"/>
-      <c r="I10" s="37"/>
-      <c r="J10" s="37"/>
-      <c r="K10" s="37"/>
-      <c r="L10" s="36"/>
+        <v>8</v>
+      </c>
+      <c r="E10" s="50"/>
+      <c r="F10" s="50"/>
+      <c r="G10" s="50"/>
+      <c r="H10" s="50"/>
+      <c r="I10" s="50"/>
+      <c r="J10" s="50"/>
+      <c r="K10" s="50"/>
+      <c r="L10" s="51"/>
       <c r="P10" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q10" s="19">
-        <v>7</v>
-      </c>
-      <c r="R10" s="19">
-        <v>22</v>
-      </c>
-      <c r="S10" s="19">
-        <v>27</v>
-      </c>
-      <c r="T10" s="19">
-        <v>72</v>
-      </c>
-      <c r="U10" s="19">
-        <v>12</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="Q10" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="R10" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="S10" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="T10" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="U10" s="17"/>
       <c r="V10" s="17"/>
       <c r="W10" s="17"/>
-      <c r="X10" s="19">
-        <v>140</v>
-      </c>
-      <c r="Y10" s="21">
-        <v>63287</v>
+      <c r="X10" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y10" s="18" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>5</v>
-      </c>
-      <c r="B11" s="36" t="s">
-        <v>14</v>
+      <c r="B11" s="37" t="s">
+        <v>16</v>
       </c>
       <c r="C11" s="33">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D11" s="34" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="38">
-        <v>7</v>
-      </c>
-      <c r="F11" s="38">
-        <v>22</v>
-      </c>
-      <c r="G11" s="38">
-        <v>27</v>
-      </c>
-      <c r="H11" s="38">
-        <v>72</v>
-      </c>
-      <c r="I11" s="38">
-        <v>12</v>
-      </c>
-      <c r="J11" s="39"/>
-      <c r="K11" s="39"/>
-      <c r="L11" s="40">
-        <v>63287</v>
-      </c>
-      <c r="P11" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="Q11" s="19">
-        <v>26</v>
-      </c>
-      <c r="R11" s="19">
-        <v>40</v>
-      </c>
-      <c r="S11" s="19">
-        <v>70</v>
-      </c>
-      <c r="T11" s="19">
-        <v>640</v>
-      </c>
-      <c r="U11" s="19">
-        <v>336</v>
-      </c>
-      <c r="V11" s="19">
-        <v>34</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="E11" s="50"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="50"/>
+      <c r="H11" s="50"/>
+      <c r="I11" s="50"/>
+      <c r="J11" s="50"/>
+      <c r="K11" s="50"/>
+      <c r="L11" s="51"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="16"/>
+      <c r="R11" s="16"/>
+      <c r="S11" s="16"/>
+      <c r="T11" s="16"/>
+      <c r="U11" s="17"/>
+      <c r="V11" s="17"/>
       <c r="W11" s="17"/>
-      <c r="X11" s="20">
-        <v>1146</v>
-      </c>
-      <c r="Y11" s="21">
-        <v>65611</v>
-      </c>
+      <c r="X11" s="16"/>
+      <c r="Y11" s="18"/>
     </row>
     <row r="12" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>5</v>
       </c>
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="35" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="33">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="D12" s="34" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="38">
-        <v>26</v>
-      </c>
-      <c r="F12" s="38">
-        <v>40</v>
-      </c>
-      <c r="G12" s="38">
-        <v>70</v>
-      </c>
-      <c r="H12" s="38">
-        <v>640</v>
-      </c>
-      <c r="I12" s="38">
-        <v>336</v>
-      </c>
-      <c r="J12" s="38">
-        <v>34</v>
-      </c>
-      <c r="K12" s="39"/>
-      <c r="L12" s="40">
-        <v>65611</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="E12" s="50"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="50"/>
+      <c r="H12" s="50"/>
+      <c r="I12" s="50"/>
+      <c r="J12" s="50"/>
+      <c r="K12" s="50"/>
+      <c r="L12" s="51"/>
       <c r="P12" s="15" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="Q12" s="19">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="R12" s="19">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="S12" s="19">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="T12" s="19">
-        <v>721</v>
-      </c>
-      <c r="U12" s="20">
-        <v>1066</v>
-      </c>
-      <c r="V12" s="19">
-        <v>774</v>
-      </c>
-      <c r="W12" s="19">
-        <v>73</v>
-      </c>
-      <c r="X12" s="20">
-        <v>2748</v>
+        <v>72</v>
+      </c>
+      <c r="U12" s="19">
+        <v>12</v>
+      </c>
+      <c r="V12" s="17"/>
+      <c r="W12" s="17"/>
+      <c r="X12" s="19">
+        <v>140</v>
       </c>
       <c r="Y12" s="21">
-        <v>66757</v>
+        <v>63287</v>
       </c>
     </row>
     <row r="13" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>5</v>
-      </c>
-      <c r="B13" s="36" t="s">
-        <v>14</v>
+      <c r="B13" s="37" t="s">
+        <v>16</v>
       </c>
       <c r="C13" s="33">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="D13" s="34" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" s="38">
-        <v>23</v>
-      </c>
-      <c r="F13" s="38">
-        <v>37</v>
-      </c>
-      <c r="G13" s="38">
-        <v>54</v>
-      </c>
-      <c r="H13" s="38">
-        <v>721</v>
-      </c>
-      <c r="I13" s="41">
-        <v>1066</v>
-      </c>
-      <c r="J13" s="38">
-        <v>774</v>
-      </c>
-      <c r="K13" s="38">
-        <v>73</v>
-      </c>
-      <c r="L13" s="40">
-        <v>66757</v>
-      </c>
-      <c r="P13" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q13" s="19">
-        <v>16</v>
-      </c>
-      <c r="R13" s="19">
-        <v>33</v>
-      </c>
-      <c r="S13" s="19">
-        <v>60</v>
-      </c>
-      <c r="T13" s="19">
-        <v>492</v>
-      </c>
-      <c r="U13" s="20">
-        <v>1097</v>
-      </c>
-      <c r="V13" s="20">
-        <v>1814</v>
-      </c>
-      <c r="W13" s="19">
-        <v>586</v>
-      </c>
-      <c r="X13" s="20">
-        <v>4098</v>
-      </c>
-      <c r="Y13" s="21">
-        <v>67641</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="E13" s="50"/>
+      <c r="F13" s="50"/>
+      <c r="G13" s="50"/>
+      <c r="H13" s="50"/>
+      <c r="I13" s="50"/>
+      <c r="J13" s="50"/>
+      <c r="K13" s="50"/>
+      <c r="L13" s="51"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="19"/>
+      <c r="R13" s="19"/>
+      <c r="S13" s="19"/>
+      <c r="T13" s="19"/>
+      <c r="U13" s="19"/>
+      <c r="V13" s="17"/>
+      <c r="W13" s="17"/>
+      <c r="X13" s="19"/>
+      <c r="Y13" s="21"/>
     </row>
     <row r="14" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>5</v>
       </c>
-      <c r="B14" s="36" t="s">
+      <c r="B14" s="35" t="s">
         <v>14</v>
       </c>
       <c r="C14" s="33">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="D14" s="34" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" s="38">
+        <v>13</v>
+      </c>
+      <c r="E14" s="48">
+        <v>7</v>
+      </c>
+      <c r="F14" s="48">
+        <v>22</v>
+      </c>
+      <c r="G14" s="48">
+        <v>27</v>
+      </c>
+      <c r="H14" s="48">
+        <v>72</v>
+      </c>
+      <c r="I14" s="48">
+        <v>12</v>
+      </c>
+      <c r="J14" s="53"/>
+      <c r="K14" s="53"/>
+      <c r="L14" s="49">
+        <v>63287</v>
+      </c>
+      <c r="P14" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q14" s="19">
+        <v>26</v>
+      </c>
+      <c r="R14" s="19">
+        <v>40</v>
+      </c>
+      <c r="S14" s="19">
+        <v>70</v>
+      </c>
+      <c r="T14" s="19">
+        <v>640</v>
+      </c>
+      <c r="U14" s="19">
+        <v>336</v>
+      </c>
+      <c r="V14" s="19">
+        <v>34</v>
+      </c>
+      <c r="W14" s="17"/>
+      <c r="X14" s="20">
+        <v>1146</v>
+      </c>
+      <c r="Y14" s="21">
+        <v>65611</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="F14" s="38">
-        <v>33</v>
-      </c>
-      <c r="G14" s="38">
-        <v>60</v>
-      </c>
-      <c r="H14" s="38">
-        <v>492</v>
-      </c>
-      <c r="I14" s="41">
-        <v>1097</v>
-      </c>
-      <c r="J14" s="41">
-        <v>1814</v>
-      </c>
-      <c r="K14" s="38">
-        <v>586</v>
-      </c>
-      <c r="L14" s="40">
-        <v>67641</v>
-      </c>
-      <c r="P14" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q14" s="19">
-        <v>15</v>
-      </c>
-      <c r="R14" s="19">
-        <v>30</v>
-      </c>
-      <c r="S14" s="19">
-        <v>68</v>
-      </c>
-      <c r="T14" s="19">
-        <v>371</v>
-      </c>
-      <c r="U14" s="19">
-        <v>762</v>
-      </c>
-      <c r="V14" s="20">
-        <v>1201</v>
-      </c>
-      <c r="W14" s="20">
-        <v>1495</v>
-      </c>
-      <c r="X14" s="20">
-        <v>3942</v>
-      </c>
-      <c r="Y14" s="21">
-        <v>66534</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>5</v>
-      </c>
-      <c r="B15" s="36" t="s">
-        <v>14</v>
-      </c>
       <c r="C15" s="33">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="D15" s="34" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15" s="38">
-        <v>15</v>
-      </c>
-      <c r="F15" s="38">
-        <v>30</v>
-      </c>
-      <c r="G15" s="38">
-        <v>68</v>
-      </c>
-      <c r="H15" s="38">
-        <v>371</v>
-      </c>
-      <c r="I15" s="38">
-        <v>762</v>
-      </c>
-      <c r="J15" s="41">
-        <v>1201</v>
-      </c>
-      <c r="K15" s="41">
-        <v>1495</v>
-      </c>
-      <c r="L15" s="40">
-        <v>66534</v>
-      </c>
-      <c r="P15" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q15" s="19">
-        <v>12</v>
-      </c>
-      <c r="R15" s="19">
-        <v>26</v>
-      </c>
-      <c r="S15" s="19">
-        <v>29</v>
-      </c>
-      <c r="T15" s="19">
-        <v>153</v>
-      </c>
-      <c r="U15" s="19">
-        <v>365</v>
-      </c>
-      <c r="V15" s="19">
-        <v>534</v>
-      </c>
-      <c r="W15" s="20">
-        <v>1099</v>
-      </c>
-      <c r="X15" s="20">
-        <v>2218</v>
-      </c>
-      <c r="Y15" s="21">
-        <v>69420</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="E15" s="48">
+        <v>63287</v>
+      </c>
+      <c r="F15" s="48">
+        <v>63287</v>
+      </c>
+      <c r="G15" s="48">
+        <v>63287</v>
+      </c>
+      <c r="H15" s="48">
+        <v>63287</v>
+      </c>
+      <c r="I15" s="48">
+        <v>63287</v>
+      </c>
+      <c r="J15" s="53"/>
+      <c r="K15" s="53"/>
+      <c r="L15" s="49"/>
+      <c r="P15" s="15"/>
+      <c r="Q15" s="19"/>
+      <c r="R15" s="19"/>
+      <c r="S15" s="19"/>
+      <c r="T15" s="19"/>
+      <c r="U15" s="19"/>
+      <c r="V15" s="19"/>
+      <c r="W15" s="17"/>
+      <c r="X15" s="20"/>
+      <c r="Y15" s="21"/>
     </row>
     <row r="16" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>5</v>
       </c>
-      <c r="B16" s="36" t="s">
+      <c r="B16" s="35" t="s">
         <v>14</v>
       </c>
       <c r="C16" s="33">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="D16" s="34" t="s">
-        <v>21</v>
-      </c>
-      <c r="E16" s="38">
-        <v>12</v>
-      </c>
-      <c r="F16" s="38">
+        <v>17</v>
+      </c>
+      <c r="E16" s="48">
         <v>26</v>
       </c>
-      <c r="G16" s="38">
-        <v>29</v>
-      </c>
-      <c r="H16" s="38">
-        <v>153</v>
-      </c>
-      <c r="I16" s="38">
-        <v>365</v>
-      </c>
-      <c r="J16" s="38">
-        <v>534</v>
-      </c>
-      <c r="K16" s="41">
-        <v>1099</v>
-      </c>
-      <c r="L16" s="40">
-        <v>69420</v>
-      </c>
+      <c r="F16" s="48">
+        <v>40</v>
+      </c>
+      <c r="G16" s="48">
+        <v>70</v>
+      </c>
+      <c r="H16" s="48">
+        <v>640</v>
+      </c>
+      <c r="I16" s="48">
+        <v>336</v>
+      </c>
+      <c r="J16" s="48">
+        <v>34</v>
+      </c>
+      <c r="K16" s="53"/>
+      <c r="L16" s="52"/>
       <c r="P16" s="15" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="Q16" s="19">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="R16" s="19">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="S16" s="19">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="T16" s="19">
-        <v>44</v>
-      </c>
-      <c r="U16" s="19">
-        <v>78</v>
+        <v>721</v>
+      </c>
+      <c r="U16" s="20">
+        <v>1066</v>
       </c>
       <c r="V16" s="19">
-        <v>111</v>
+        <v>774</v>
       </c>
       <c r="W16" s="19">
-        <v>282</v>
-      </c>
-      <c r="X16" s="19">
-        <v>536</v>
+        <v>73</v>
+      </c>
+      <c r="X16" s="20">
+        <v>2748</v>
       </c>
       <c r="Y16" s="21">
-        <v>72259</v>
+        <v>66757</v>
       </c>
     </row>
     <row r="17" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>5</v>
-      </c>
-      <c r="B17" s="36" t="s">
-        <v>14</v>
+      <c r="B17" s="37" t="s">
+        <v>16</v>
       </c>
       <c r="C17" s="33">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="D17" s="34" t="s">
-        <v>22</v>
-      </c>
-      <c r="E17" s="38">
-        <v>3</v>
-      </c>
-      <c r="F17" s="38">
-        <v>6</v>
-      </c>
-      <c r="G17" s="38">
-        <v>12</v>
-      </c>
-      <c r="H17" s="38">
-        <v>44</v>
-      </c>
-      <c r="I17" s="38">
-        <v>78</v>
-      </c>
-      <c r="J17" s="38">
-        <v>111</v>
-      </c>
-      <c r="K17" s="38">
-        <v>282</v>
-      </c>
-      <c r="L17" s="40">
-        <v>72259</v>
-      </c>
-      <c r="P17" s="22" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q17" s="23">
-        <v>3</v>
-      </c>
-      <c r="R17" s="23">
-        <v>4</v>
-      </c>
-      <c r="S17" s="23">
-        <v>1</v>
-      </c>
-      <c r="T17" s="23">
-        <v>8</v>
-      </c>
-      <c r="U17" s="23">
-        <v>13</v>
-      </c>
-      <c r="V17" s="23">
-        <v>20</v>
-      </c>
-      <c r="W17" s="23">
-        <v>108</v>
-      </c>
-      <c r="X17" s="23">
-        <v>157</v>
-      </c>
-      <c r="Y17" s="24">
-        <v>72048</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="E17" s="48">
+        <v>65611</v>
+      </c>
+      <c r="F17" s="48">
+        <v>65611</v>
+      </c>
+      <c r="G17" s="48">
+        <v>65611</v>
+      </c>
+      <c r="H17" s="48">
+        <v>65611</v>
+      </c>
+      <c r="I17" s="48">
+        <v>65611</v>
+      </c>
+      <c r="J17" s="48">
+        <v>65611</v>
+      </c>
+      <c r="K17" s="48">
+        <v>65611</v>
+      </c>
+      <c r="L17" s="49">
+        <v>65611</v>
+      </c>
+      <c r="P17" s="15"/>
+      <c r="Q17" s="19"/>
+      <c r="R17" s="19"/>
+      <c r="S17" s="19"/>
+      <c r="T17" s="19"/>
+      <c r="U17" s="20"/>
+      <c r="V17" s="19"/>
+      <c r="W17" s="19"/>
+      <c r="X17" s="20"/>
+      <c r="Y17" s="21"/>
     </row>
     <row r="18" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>5</v>
       </c>
-      <c r="B18" s="36" t="s">
+      <c r="B18" s="35" t="s">
         <v>14</v>
       </c>
       <c r="C18" s="33">
+        <v>47</v>
+      </c>
+      <c r="D18" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="48">
+        <v>23</v>
+      </c>
+      <c r="F18" s="48">
+        <v>37</v>
+      </c>
+      <c r="G18" s="48">
+        <v>54</v>
+      </c>
+      <c r="H18" s="48">
+        <v>721</v>
+      </c>
+      <c r="I18" s="48">
+        <v>1066</v>
+      </c>
+      <c r="J18" s="48">
+        <v>774</v>
+      </c>
+      <c r="K18" s="48">
+        <v>73</v>
+      </c>
+      <c r="L18" s="49"/>
+      <c r="P18" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q18" s="19">
+        <v>16</v>
+      </c>
+      <c r="R18" s="19">
+        <v>33</v>
+      </c>
+      <c r="S18" s="19">
+        <v>60</v>
+      </c>
+      <c r="T18" s="19">
+        <v>492</v>
+      </c>
+      <c r="U18" s="20">
+        <v>1097</v>
+      </c>
+      <c r="V18" s="20">
+        <v>1814</v>
+      </c>
+      <c r="W18" s="19">
+        <v>586</v>
+      </c>
+      <c r="X18" s="20">
+        <v>4098</v>
+      </c>
+      <c r="Y18" s="21">
+        <v>67641</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B19" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="33">
+        <v>47</v>
+      </c>
+      <c r="D19" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="48">
+        <v>66757</v>
+      </c>
+      <c r="F19" s="48">
+        <v>66757</v>
+      </c>
+      <c r="G19" s="48">
+        <v>66757</v>
+      </c>
+      <c r="H19" s="48">
+        <v>66757</v>
+      </c>
+      <c r="I19" s="48">
+        <v>66757</v>
+      </c>
+      <c r="J19" s="48">
+        <v>66757</v>
+      </c>
+      <c r="K19" s="48">
+        <v>66757</v>
+      </c>
+      <c r="L19" s="49">
+        <v>66757</v>
+      </c>
+      <c r="P19" s="15"/>
+      <c r="Q19" s="19"/>
+      <c r="R19" s="19"/>
+      <c r="S19" s="19"/>
+      <c r="T19" s="19"/>
+      <c r="U19" s="20"/>
+      <c r="V19" s="20"/>
+      <c r="W19" s="19"/>
+      <c r="X19" s="20"/>
+      <c r="Y19" s="21"/>
+    </row>
+    <row r="20" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>5</v>
+      </c>
+      <c r="B20" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="33">
+        <v>52</v>
+      </c>
+      <c r="D20" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" s="48">
+        <v>16</v>
+      </c>
+      <c r="F20" s="48">
+        <v>33</v>
+      </c>
+      <c r="G20" s="48">
+        <v>60</v>
+      </c>
+      <c r="H20" s="48">
+        <v>492</v>
+      </c>
+      <c r="I20" s="48">
+        <v>1097</v>
+      </c>
+      <c r="J20" s="48">
+        <v>1814</v>
+      </c>
+      <c r="K20" s="48">
+        <v>586</v>
+      </c>
+      <c r="L20" s="49"/>
+      <c r="P20" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q20" s="19">
+        <v>15</v>
+      </c>
+      <c r="R20" s="19">
+        <v>30</v>
+      </c>
+      <c r="S20" s="19">
+        <v>68</v>
+      </c>
+      <c r="T20" s="19">
+        <v>371</v>
+      </c>
+      <c r="U20" s="19">
+        <v>762</v>
+      </c>
+      <c r="V20" s="20">
+        <v>1201</v>
+      </c>
+      <c r="W20" s="20">
+        <v>1495</v>
+      </c>
+      <c r="X20" s="20">
+        <v>3942</v>
+      </c>
+      <c r="Y20" s="21">
+        <v>66534</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B21" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="33">
+        <v>52</v>
+      </c>
+      <c r="D21" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" s="48">
+        <v>67641</v>
+      </c>
+      <c r="F21" s="48">
+        <v>67641</v>
+      </c>
+      <c r="G21" s="48">
+        <v>67641</v>
+      </c>
+      <c r="H21" s="48">
+        <v>67641</v>
+      </c>
+      <c r="I21" s="48">
+        <v>67641</v>
+      </c>
+      <c r="J21" s="48">
+        <v>67641</v>
+      </c>
+      <c r="K21" s="48">
+        <v>67641</v>
+      </c>
+      <c r="L21" s="49">
+        <v>67641</v>
+      </c>
+      <c r="P21" s="15"/>
+      <c r="Q21" s="19"/>
+      <c r="R21" s="19"/>
+      <c r="S21" s="19"/>
+      <c r="T21" s="19"/>
+      <c r="U21" s="19"/>
+      <c r="V21" s="20"/>
+      <c r="W21" s="20"/>
+      <c r="X21" s="20"/>
+      <c r="Y21" s="21"/>
+    </row>
+    <row r="22" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>5</v>
+      </c>
+      <c r="B22" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="33">
+        <v>57</v>
+      </c>
+      <c r="D22" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="E22" s="48">
+        <v>15</v>
+      </c>
+      <c r="F22" s="48">
+        <v>30</v>
+      </c>
+      <c r="G22" s="48">
+        <v>68</v>
+      </c>
+      <c r="H22" s="48">
+        <v>371</v>
+      </c>
+      <c r="I22" s="48">
+        <v>762</v>
+      </c>
+      <c r="J22" s="48">
+        <v>1201</v>
+      </c>
+      <c r="K22" s="48">
+        <v>1495</v>
+      </c>
+      <c r="L22" s="49"/>
+      <c r="P22" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q22" s="19">
+        <v>12</v>
+      </c>
+      <c r="R22" s="19">
+        <v>26</v>
+      </c>
+      <c r="S22" s="19">
+        <v>29</v>
+      </c>
+      <c r="T22" s="19">
+        <v>153</v>
+      </c>
+      <c r="U22" s="19">
+        <v>365</v>
+      </c>
+      <c r="V22" s="19">
+        <v>534</v>
+      </c>
+      <c r="W22" s="20">
+        <v>1099</v>
+      </c>
+      <c r="X22" s="20">
+        <v>2218</v>
+      </c>
+      <c r="Y22" s="21">
+        <v>69420</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B23" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" s="33">
+        <v>57</v>
+      </c>
+      <c r="D23" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="E23" s="48">
+        <v>66534</v>
+      </c>
+      <c r="F23" s="48">
+        <v>66534</v>
+      </c>
+      <c r="G23" s="48">
+        <v>66534</v>
+      </c>
+      <c r="H23" s="48">
+        <v>66534</v>
+      </c>
+      <c r="I23" s="48">
+        <v>66534</v>
+      </c>
+      <c r="J23" s="48">
+        <v>66534</v>
+      </c>
+      <c r="K23" s="48">
+        <v>66534</v>
+      </c>
+      <c r="L23" s="49">
+        <v>66534</v>
+      </c>
+      <c r="P23" s="15"/>
+      <c r="Q23" s="19"/>
+      <c r="R23" s="19"/>
+      <c r="S23" s="19"/>
+      <c r="T23" s="19"/>
+      <c r="U23" s="19"/>
+      <c r="V23" s="19"/>
+      <c r="W23" s="20"/>
+      <c r="X23" s="20"/>
+      <c r="Y23" s="21"/>
+    </row>
+    <row r="24" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>5</v>
+      </c>
+      <c r="B24" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="33">
+        <v>62</v>
+      </c>
+      <c r="D24" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" s="48">
+        <v>12</v>
+      </c>
+      <c r="F24" s="48">
+        <v>26</v>
+      </c>
+      <c r="G24" s="48">
+        <v>29</v>
+      </c>
+      <c r="H24" s="48">
+        <v>153</v>
+      </c>
+      <c r="I24" s="48">
+        <v>365</v>
+      </c>
+      <c r="J24" s="48">
+        <v>534</v>
+      </c>
+      <c r="K24" s="48">
+        <v>1099</v>
+      </c>
+      <c r="L24" s="49"/>
+      <c r="P24" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q24" s="19">
+        <v>3</v>
+      </c>
+      <c r="R24" s="19">
+        <v>6</v>
+      </c>
+      <c r="S24" s="19">
+        <v>12</v>
+      </c>
+      <c r="T24" s="19">
+        <v>44</v>
+      </c>
+      <c r="U24" s="19">
+        <v>78</v>
+      </c>
+      <c r="V24" s="19">
+        <v>111</v>
+      </c>
+      <c r="W24" s="19">
+        <v>282</v>
+      </c>
+      <c r="X24" s="19">
+        <v>536</v>
+      </c>
+      <c r="Y24" s="21">
+        <v>72259</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B25" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="33">
+        <v>62</v>
+      </c>
+      <c r="D25" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25" s="48">
+        <v>69420</v>
+      </c>
+      <c r="F25" s="48">
+        <v>69420</v>
+      </c>
+      <c r="G25" s="48">
+        <v>69420</v>
+      </c>
+      <c r="H25" s="48">
+        <v>69420</v>
+      </c>
+      <c r="I25" s="48">
+        <v>69420</v>
+      </c>
+      <c r="J25" s="48">
+        <v>69420</v>
+      </c>
+      <c r="K25" s="48">
+        <v>69420</v>
+      </c>
+      <c r="L25" s="49">
+        <v>69420</v>
+      </c>
+      <c r="P25" s="15"/>
+      <c r="Q25" s="19"/>
+      <c r="R25" s="19"/>
+      <c r="S25" s="19"/>
+      <c r="T25" s="19"/>
+      <c r="U25" s="19"/>
+      <c r="V25" s="19"/>
+      <c r="W25" s="19"/>
+      <c r="X25" s="19"/>
+      <c r="Y25" s="21"/>
+    </row>
+    <row r="26" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>5</v>
+      </c>
+      <c r="B26" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="33">
+        <v>67</v>
+      </c>
+      <c r="D26" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="E26" s="48">
+        <v>3</v>
+      </c>
+      <c r="F26" s="48">
+        <v>6</v>
+      </c>
+      <c r="G26" s="48">
+        <v>12</v>
+      </c>
+      <c r="H26" s="48">
+        <v>44</v>
+      </c>
+      <c r="I26" s="48">
+        <v>78</v>
+      </c>
+      <c r="J26" s="48">
+        <v>111</v>
+      </c>
+      <c r="K26" s="48">
+        <v>282</v>
+      </c>
+      <c r="L26" s="49"/>
+      <c r="P26" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q26" s="23">
+        <v>3</v>
+      </c>
+      <c r="R26" s="23">
+        <v>4</v>
+      </c>
+      <c r="S26" s="23">
+        <v>1</v>
+      </c>
+      <c r="T26" s="23">
+        <v>8</v>
+      </c>
+      <c r="U26" s="23">
+        <v>13</v>
+      </c>
+      <c r="V26" s="23">
+        <v>20</v>
+      </c>
+      <c r="W26" s="23">
+        <v>108</v>
+      </c>
+      <c r="X26" s="23">
+        <v>157</v>
+      </c>
+      <c r="Y26" s="24">
+        <v>72048</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B27" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" s="33">
+        <v>67</v>
+      </c>
+      <c r="D27" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27" s="48">
+        <v>72259</v>
+      </c>
+      <c r="F27" s="48">
+        <v>72259</v>
+      </c>
+      <c r="G27" s="48">
+        <v>72259</v>
+      </c>
+      <c r="H27" s="48">
+        <v>72259</v>
+      </c>
+      <c r="I27" s="48">
+        <v>72259</v>
+      </c>
+      <c r="J27" s="48">
+        <v>72259</v>
+      </c>
+      <c r="K27" s="48">
+        <v>72259</v>
+      </c>
+      <c r="L27" s="49">
+        <v>72259</v>
+      </c>
+      <c r="P27" s="22"/>
+      <c r="Q27" s="23"/>
+      <c r="R27" s="23"/>
+      <c r="S27" s="23"/>
+      <c r="T27" s="23"/>
+      <c r="U27" s="23"/>
+      <c r="V27" s="23"/>
+      <c r="W27" s="23"/>
+      <c r="X27" s="23"/>
+      <c r="Y27" s="24"/>
+    </row>
+    <row r="28" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>5</v>
+      </c>
+      <c r="B28" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" s="33">
         <v>72</v>
       </c>
-      <c r="D18" s="34" t="s">
+      <c r="D28" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="E18" s="38">
+      <c r="E28" s="48">
         <v>3</v>
       </c>
-      <c r="F18" s="38">
+      <c r="F28" s="48">
         <v>4</v>
       </c>
-      <c r="G18" s="38">
+      <c r="G28" s="48">
         <v>1</v>
       </c>
-      <c r="H18" s="38">
+      <c r="H28" s="48">
         <v>8</v>
       </c>
-      <c r="I18" s="38">
+      <c r="I28" s="48">
         <v>13</v>
       </c>
-      <c r="J18" s="38">
+      <c r="J28" s="48">
         <v>20</v>
       </c>
-      <c r="K18" s="38">
+      <c r="K28" s="48">
         <v>108</v>
       </c>
-      <c r="L18" s="40">
+      <c r="L28" s="49"/>
+      <c r="P28" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q28" s="26">
+        <v>105</v>
+      </c>
+      <c r="R28" s="26">
+        <v>198</v>
+      </c>
+      <c r="S28" s="26">
+        <v>321</v>
+      </c>
+      <c r="T28" s="27">
+        <v>2501</v>
+      </c>
+      <c r="U28" s="27">
+        <v>3729</v>
+      </c>
+      <c r="V28" s="27">
+        <v>4488</v>
+      </c>
+      <c r="W28" s="27">
+        <v>3643</v>
+      </c>
+      <c r="X28" s="27">
+        <v>14985</v>
+      </c>
+      <c r="Y28" s="28">
+        <v>67467</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B29" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" s="33">
+        <v>72</v>
+      </c>
+      <c r="D29" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="E29" s="48">
         <v>72048</v>
       </c>
-      <c r="P18" s="25" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q18" s="26">
-        <v>105</v>
-      </c>
-      <c r="R18" s="26">
-        <v>198</v>
-      </c>
-      <c r="S18" s="26">
-        <v>321</v>
-      </c>
-      <c r="T18" s="27">
-        <v>2501</v>
-      </c>
-      <c r="U18" s="27">
-        <v>3729</v>
-      </c>
-      <c r="V18" s="27">
-        <v>4488</v>
-      </c>
-      <c r="W18" s="27">
-        <v>3643</v>
-      </c>
-      <c r="X18" s="27">
-        <v>14985</v>
-      </c>
-      <c r="Y18" s="28">
-        <v>67467</v>
-      </c>
-    </row>
-    <row r="19" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="L19" s="35"/>
+      <c r="F29" s="48">
+        <v>72048</v>
+      </c>
+      <c r="G29" s="48">
+        <v>72048</v>
+      </c>
+      <c r="H29" s="48">
+        <v>72048</v>
+      </c>
+      <c r="I29" s="48">
+        <v>72048</v>
+      </c>
+      <c r="J29" s="48">
+        <v>72048</v>
+      </c>
+      <c r="K29" s="48">
+        <v>72048</v>
+      </c>
+      <c r="L29" s="49">
+        <v>72048</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3139,7 +3669,8 @@
     <hyperlink ref="A1" location="TOC!A1" display="TOC"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3148,7 +3679,7 @@
   <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:K28"/>
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
update for prelim runs
</commit_message>
<xml_diff>
--- a/Data_inputs/MISERS_MemberData.xlsx
+++ b/Data_inputs/MISERS_MemberData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17030"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="5" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="9" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="TOC" sheetId="20" r:id="rId1"/>
@@ -17,8 +17,11 @@
     <sheet name="Actives_t1.num_CRR2013" sheetId="27" r:id="rId8"/>
     <sheet name="Actives_t1.sal_CRR2013" sheetId="28" r:id="rId9"/>
     <sheet name="RetBen_t1_AV2014" sheetId="30" r:id="rId10"/>
-    <sheet name="RetBen_t1_CRR2013" sheetId="31" r:id="rId11"/>
-    <sheet name="Sheet1" sheetId="36" r:id="rId12"/>
+    <sheet name="RetBen_t1_CRR2013_original" sheetId="31" r:id="rId11"/>
+    <sheet name="RetBen_t1_CRR2013_shifted1" sheetId="38" r:id="rId12"/>
+    <sheet name="RetBen_t1_CRR2013_shifted2" sheetId="39" r:id="rId13"/>
+    <sheet name="RetBen_t1_CRR2013" sheetId="40" r:id="rId14"/>
+    <sheet name="Sheet1" sheetId="36" r:id="rId15"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -30,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="118">
   <si>
     <t>TOC</t>
   </si>
@@ -569,6 +572,21 @@
   </si>
   <si>
     <t>factor</t>
+  </si>
+  <si>
+    <t>85-89</t>
+  </si>
+  <si>
+    <t>90-94</t>
+  </si>
+  <si>
+    <t>95-99</t>
+  </si>
+  <si>
+    <t>100-104</t>
+  </si>
+  <si>
+    <t>105-109</t>
   </si>
 </sst>
 </file>
@@ -950,6 +968,216 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>437976</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>94912</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9134475" y="1581150"/>
+          <a:ext cx="1533351" cy="2704762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>76031</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>152055</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10896600" y="1581150"/>
+          <a:ext cx="1638131" cy="2761905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>914400</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5876925" y="1257300"/>
+          <a:ext cx="2762250" cy="3962400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Notes:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>- The total number of retirees</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> and beneficiaries 32,394 does not match the number in AV2014, 56,852 (p D-2). One possible reason is that it does not include disability and death benefit of tier 2 (DC) mambers. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>- Average benefits each cell are the same. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>- 25 does not look a correct starting age. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>- Known values:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> - Total year-1 number of retirees: 57615</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> - Total year-1 benefit payment: 1,222m </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1343,6 +1571,450 @@
           <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
         </a:p>
         <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>- Known values:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> - Total year-1 number of retirees: 57615</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> - Total year-1 benefit payment: 1,222m </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>437976</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>94912</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9134475" y="1581150"/>
+          <a:ext cx="1533351" cy="2704762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>76031</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>152055</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10896600" y="1581150"/>
+          <a:ext cx="1638131" cy="2761905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>914400</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5876925" y="1257300"/>
+          <a:ext cx="2762250" cy="3962400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Notes:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>- The total number of retirees</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> and beneficiaries 32,394 does not match the number in AV2014, 56,852 (p D-2). One possible reason is that it does not include disability and death benefit of tier 2 (DC) mambers. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>- Average benefits each cell are the same. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>- 25 does not look a correct starting age. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>- Known values:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> - Total year-1 number of retirees: 57615</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> - Total year-1 benefit payment: 1,222m </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>437976</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>94912</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9134475" y="1581150"/>
+          <a:ext cx="1533351" cy="2704762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>76031</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>152055</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10896600" y="1581150"/>
+          <a:ext cx="1638131" cy="2761905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>914400</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5876925" y="1257300"/>
+          <a:ext cx="2762250" cy="3962400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Notes:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>- The total number of retirees</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> and beneficiaries 32,394 does not match the number in AV2014, 56,852 (p D-2). One possible reason is that it does not include disability and death benefit of tier 2 (DC) mambers. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>- Average benefits each cell are the same. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>- 25 does not look a correct starting age. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>- Known values:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> - Total year-1 number of retirees: 57615</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> - Total year-1 benefit payment: 1,222m </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
             <a:t> </a:t>
@@ -1664,8 +2336,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1847,9 +2519,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="10" max="10" width="18.28515625" customWidth="1"/>
-    <col min="11" max="13" width="14.5703125" customWidth="1"/>
-    <col min="14" max="14" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.25" customWidth="1"/>
+    <col min="11" max="13" width="14.625" customWidth="1"/>
+    <col min="14" max="14" width="9.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -1910,17 +2582,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="9.140625" customWidth="1"/>
+    <col min="1" max="3" width="9.125" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.28515625" customWidth="1"/>
-    <col min="13" max="15" width="14.5703125" customWidth="1"/>
-    <col min="16" max="16" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.25" customWidth="1"/>
+    <col min="13" max="15" width="14.625" customWidth="1"/>
+    <col min="16" max="16" width="9.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
@@ -2333,6 +3005,1284 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="9.125" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.25" customWidth="1"/>
+    <col min="13" max="15" width="14.625" customWidth="1"/>
+    <col min="16" max="16" width="9.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="P1" s="1"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="P2" s="2"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="P3" s="2"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="P4" s="2"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="P5" s="2"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="P6" s="2"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>40</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="29">
+        <v>42</v>
+      </c>
+      <c r="D9" s="29">
+        <v>533</v>
+      </c>
+      <c r="E9" s="29">
+        <f>F9/D9</f>
+        <v>1615.7913193245779</v>
+      </c>
+      <c r="F9">
+        <v>861216.77320000005</v>
+      </c>
+      <c r="G9">
+        <f>E9*12</f>
+        <v>19389.495831894936</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="29">
+        <v>47</v>
+      </c>
+      <c r="D10" s="29">
+        <v>1010</v>
+      </c>
+      <c r="E10" s="29">
+        <f t="shared" ref="E10:E20" si="0">F10/D10</f>
+        <v>1615.7913198019803</v>
+      </c>
+      <c r="F10">
+        <v>1631949.233</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="29">
+        <v>52</v>
+      </c>
+      <c r="D11" s="29">
+        <v>3503</v>
+      </c>
+      <c r="E11" s="29">
+        <f t="shared" si="0"/>
+        <v>1615.7913194404796</v>
+      </c>
+      <c r="F11">
+        <v>5660116.9919999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="29">
+        <v>57</v>
+      </c>
+      <c r="D12" s="29">
+        <v>7419</v>
+      </c>
+      <c r="E12" s="29">
+        <f t="shared" si="0"/>
+        <v>1615.7913195848498</v>
+      </c>
+      <c r="F12">
+        <v>11987555.800000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="29">
+        <v>62</v>
+      </c>
+      <c r="D13" s="29">
+        <v>6631</v>
+      </c>
+      <c r="E13" s="29">
+        <f t="shared" si="0"/>
+        <v>1615.7913195596441</v>
+      </c>
+      <c r="F13">
+        <v>10714312.24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="29">
+        <v>67</v>
+      </c>
+      <c r="D14" s="29">
+        <v>4813</v>
+      </c>
+      <c r="E14" s="29">
+        <f t="shared" si="0"/>
+        <v>1615.7913193434449</v>
+      </c>
+      <c r="F14">
+        <v>7776803.6200000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="29">
+        <v>72</v>
+      </c>
+      <c r="D15" s="29">
+        <v>3457</v>
+      </c>
+      <c r="E15" s="29">
+        <f t="shared" si="0"/>
+        <v>1615.7913193520394</v>
+      </c>
+      <c r="F15">
+        <v>5585790.591</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" s="29">
+        <v>77</v>
+      </c>
+      <c r="D16" s="29">
+        <v>2455</v>
+      </c>
+      <c r="E16" s="29">
+        <f t="shared" si="0"/>
+        <v>1615.7913193482686</v>
+      </c>
+      <c r="F16">
+        <v>3966767.6889999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>5</v>
+      </c>
+      <c r="B17" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" s="29">
+        <v>82</v>
+      </c>
+      <c r="D17" s="29">
+        <v>1626</v>
+      </c>
+      <c r="E17" s="29">
+        <f t="shared" si="0"/>
+        <v>1615.7913191881919</v>
+      </c>
+      <c r="F17">
+        <v>2627276.6850000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>113</v>
+      </c>
+      <c r="C18" s="29">
+        <v>87</v>
+      </c>
+      <c r="D18" s="29">
+        <v>731</v>
+      </c>
+      <c r="E18" s="29">
+        <f t="shared" si="0"/>
+        <v>1615.7913187414499</v>
+      </c>
+      <c r="F18">
+        <v>1181143.4539999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>5</v>
+      </c>
+      <c r="B19" t="s">
+        <v>114</v>
+      </c>
+      <c r="C19" s="29">
+        <v>92</v>
+      </c>
+      <c r="D19" s="29">
+        <v>201</v>
+      </c>
+      <c r="E19" s="29">
+        <f t="shared" si="0"/>
+        <v>1615.791319402985</v>
+      </c>
+      <c r="F19">
+        <v>324774.0552</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>5</v>
+      </c>
+      <c r="B20" t="s">
+        <v>115</v>
+      </c>
+      <c r="C20" s="29">
+        <v>97</v>
+      </c>
+      <c r="D20" s="29">
+        <v>15</v>
+      </c>
+      <c r="E20" s="29">
+        <f t="shared" si="0"/>
+        <v>1615.7913193333334</v>
+      </c>
+      <c r="F20">
+        <v>24236.869790000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <f>57615/32394</f>
+        <v>1.7785701055751064</v>
+      </c>
+      <c r="F24">
+        <f>53241944*D24 *12</f>
+        <v>1136334359.5332468</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" location="TOC!A1" display="TOC"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="9.125" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.25" customWidth="1"/>
+    <col min="13" max="15" width="14.625" customWidth="1"/>
+    <col min="16" max="16" width="9.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="P1" s="1"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="P2" s="2"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="P3" s="2"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="P4" s="2"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="P5" s="2"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="P6" s="2"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>40</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="29">
+        <v>52</v>
+      </c>
+      <c r="D9" s="29">
+        <v>533</v>
+      </c>
+      <c r="E9" s="29">
+        <f>F9/D9</f>
+        <v>1615.7913193245779</v>
+      </c>
+      <c r="F9">
+        <v>861216.77320000005</v>
+      </c>
+      <c r="G9">
+        <f>E9*12</f>
+        <v>19389.495831894936</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="29">
+        <v>57</v>
+      </c>
+      <c r="D10" s="29">
+        <v>1010</v>
+      </c>
+      <c r="E10" s="29">
+        <f t="shared" ref="E10:E20" si="0">F10/D10</f>
+        <v>1615.7913198019803</v>
+      </c>
+      <c r="F10">
+        <v>1631949.233</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="29">
+        <v>62</v>
+      </c>
+      <c r="D11" s="29">
+        <v>3503</v>
+      </c>
+      <c r="E11" s="29">
+        <f t="shared" si="0"/>
+        <v>1615.7913194404796</v>
+      </c>
+      <c r="F11">
+        <v>5660116.9919999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="29">
+        <v>67</v>
+      </c>
+      <c r="D12" s="29">
+        <v>7419</v>
+      </c>
+      <c r="E12" s="29">
+        <f t="shared" si="0"/>
+        <v>1615.7913195848498</v>
+      </c>
+      <c r="F12">
+        <v>11987555.800000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="29">
+        <v>72</v>
+      </c>
+      <c r="D13" s="29">
+        <v>6631</v>
+      </c>
+      <c r="E13" s="29">
+        <f t="shared" si="0"/>
+        <v>1615.7913195596441</v>
+      </c>
+      <c r="F13">
+        <v>10714312.24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" s="29">
+        <v>77</v>
+      </c>
+      <c r="D14" s="29">
+        <v>4813</v>
+      </c>
+      <c r="E14" s="29">
+        <f t="shared" si="0"/>
+        <v>1615.7913193434449</v>
+      </c>
+      <c r="F14">
+        <v>7776803.6200000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" s="29">
+        <v>82</v>
+      </c>
+      <c r="D15" s="29">
+        <v>3457</v>
+      </c>
+      <c r="E15" s="29">
+        <f t="shared" si="0"/>
+        <v>1615.7913193520394</v>
+      </c>
+      <c r="F15">
+        <v>5585790.591</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>113</v>
+      </c>
+      <c r="C16" s="29">
+        <v>87</v>
+      </c>
+      <c r="D16" s="29">
+        <v>2455</v>
+      </c>
+      <c r="E16" s="29">
+        <f t="shared" si="0"/>
+        <v>1615.7913193482686</v>
+      </c>
+      <c r="F16">
+        <v>3966767.6889999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>5</v>
+      </c>
+      <c r="B17" t="s">
+        <v>114</v>
+      </c>
+      <c r="C17" s="29">
+        <v>92</v>
+      </c>
+      <c r="D17" s="29">
+        <v>1626</v>
+      </c>
+      <c r="E17" s="29">
+        <f t="shared" si="0"/>
+        <v>1615.7913191881919</v>
+      </c>
+      <c r="F17">
+        <v>2627276.6850000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>115</v>
+      </c>
+      <c r="C18" s="29">
+        <v>97</v>
+      </c>
+      <c r="D18" s="29">
+        <v>731</v>
+      </c>
+      <c r="E18" s="29">
+        <f t="shared" si="0"/>
+        <v>1615.7913187414499</v>
+      </c>
+      <c r="F18">
+        <v>1181143.4539999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>5</v>
+      </c>
+      <c r="B19" t="s">
+        <v>116</v>
+      </c>
+      <c r="C19" s="29">
+        <v>102</v>
+      </c>
+      <c r="D19" s="29">
+        <v>201</v>
+      </c>
+      <c r="E19" s="29">
+        <f t="shared" si="0"/>
+        <v>1615.791319402985</v>
+      </c>
+      <c r="F19">
+        <v>324774.0552</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>5</v>
+      </c>
+      <c r="B20" t="s">
+        <v>117</v>
+      </c>
+      <c r="C20" s="29">
+        <v>107</v>
+      </c>
+      <c r="D20" s="29">
+        <v>15</v>
+      </c>
+      <c r="E20" s="29">
+        <f t="shared" si="0"/>
+        <v>1615.7913193333334</v>
+      </c>
+      <c r="F20">
+        <v>24236.869790000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <f>57615/32394</f>
+        <v>1.7785701055751064</v>
+      </c>
+      <c r="F24">
+        <f>53241944*D24 *12</f>
+        <v>1136334359.5332468</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" location="TOC!A1" display="TOC"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="9.125" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.25" customWidth="1"/>
+    <col min="13" max="15" width="14.625" customWidth="1"/>
+    <col min="16" max="16" width="9.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="P1" s="1"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="P2" s="2"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="P3" s="2"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="P4" s="2"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="P5" s="2"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="P6" s="2"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>40</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9">
+        <v>47</v>
+      </c>
+      <c r="D9" s="29">
+        <v>533</v>
+      </c>
+      <c r="E9" s="29">
+        <f>F9/D9</f>
+        <v>1615.7913193245779</v>
+      </c>
+      <c r="F9">
+        <v>861216.77320000005</v>
+      </c>
+      <c r="G9">
+        <f>E9*12</f>
+        <v>19389.495831894936</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="29">
+        <v>52</v>
+      </c>
+      <c r="D10" s="29">
+        <v>1010</v>
+      </c>
+      <c r="E10" s="29">
+        <f t="shared" ref="E10:E20" si="0">F10/D10</f>
+        <v>1615.7913198019803</v>
+      </c>
+      <c r="F10">
+        <v>1631949.233</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="29">
+        <v>57</v>
+      </c>
+      <c r="D11" s="29">
+        <v>3503</v>
+      </c>
+      <c r="E11" s="29">
+        <f t="shared" si="0"/>
+        <v>1615.7913194404796</v>
+      </c>
+      <c r="F11">
+        <v>5660116.9919999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="29">
+        <v>62</v>
+      </c>
+      <c r="D12" s="29">
+        <v>7419</v>
+      </c>
+      <c r="E12" s="29">
+        <f t="shared" si="0"/>
+        <v>1615.7913195848498</v>
+      </c>
+      <c r="F12">
+        <v>11987555.800000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="29">
+        <v>67</v>
+      </c>
+      <c r="D13" s="29">
+        <v>6631</v>
+      </c>
+      <c r="E13" s="29">
+        <f t="shared" si="0"/>
+        <v>1615.7913195596441</v>
+      </c>
+      <c r="F13">
+        <v>10714312.24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" s="29">
+        <v>72</v>
+      </c>
+      <c r="D14" s="29">
+        <v>4813</v>
+      </c>
+      <c r="E14" s="29">
+        <f t="shared" si="0"/>
+        <v>1615.7913193434449</v>
+      </c>
+      <c r="F14">
+        <v>7776803.6200000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" s="29">
+        <v>77</v>
+      </c>
+      <c r="D15" s="29">
+        <v>3457</v>
+      </c>
+      <c r="E15" s="29">
+        <f t="shared" si="0"/>
+        <v>1615.7913193520394</v>
+      </c>
+      <c r="F15">
+        <v>5585790.591</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="29">
+        <v>82</v>
+      </c>
+      <c r="D16" s="29">
+        <v>2455</v>
+      </c>
+      <c r="E16" s="29">
+        <f t="shared" si="0"/>
+        <v>1615.7913193482686</v>
+      </c>
+      <c r="F16">
+        <v>3966767.6889999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>5</v>
+      </c>
+      <c r="B17" t="s">
+        <v>113</v>
+      </c>
+      <c r="C17" s="29">
+        <v>87</v>
+      </c>
+      <c r="D17" s="29">
+        <v>1626</v>
+      </c>
+      <c r="E17" s="29">
+        <f t="shared" si="0"/>
+        <v>1615.7913191881919</v>
+      </c>
+      <c r="F17">
+        <v>2627276.6850000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>114</v>
+      </c>
+      <c r="C18" s="29">
+        <v>92</v>
+      </c>
+      <c r="D18" s="29">
+        <v>731</v>
+      </c>
+      <c r="E18" s="29">
+        <f t="shared" si="0"/>
+        <v>1615.7913187414499</v>
+      </c>
+      <c r="F18">
+        <v>1181143.4539999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>5</v>
+      </c>
+      <c r="B19" t="s">
+        <v>115</v>
+      </c>
+      <c r="C19" s="29">
+        <v>97</v>
+      </c>
+      <c r="D19" s="29">
+        <v>201</v>
+      </c>
+      <c r="E19" s="29">
+        <f t="shared" si="0"/>
+        <v>1615.791319402985</v>
+      </c>
+      <c r="F19">
+        <v>324774.0552</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>5</v>
+      </c>
+      <c r="B20" t="s">
+        <v>116</v>
+      </c>
+      <c r="C20" s="29">
+        <v>102</v>
+      </c>
+      <c r="D20" s="29">
+        <v>15</v>
+      </c>
+      <c r="E20" s="29">
+        <f t="shared" si="0"/>
+        <v>1615.7913193333334</v>
+      </c>
+      <c r="F20">
+        <v>24236.869790000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C21" s="29"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <f>57615/32394</f>
+        <v>1.7785701055751064</v>
+      </c>
+      <c r="F24">
+        <f>53241944*D24 *12</f>
+        <v>1136334359.5332468</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" location="TOC!A1" display="TOC"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:Y21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2341,7 +4291,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="12" max="12" width="17.42578125" customWidth="1"/>
+    <col min="12" max="12" width="17.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:25" x14ac:dyDescent="0.25">
@@ -3538,8 +5488,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.375" customWidth="1"/>
+    <col min="4" max="4" width="12.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -3736,15 +5686,15 @@
   <dimension ref="A1:Y29"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8:L29"/>
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="12" width="15.42578125" style="40" customWidth="1"/>
-    <col min="13" max="13" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.28515625" customWidth="1"/>
-    <col min="25" max="25" width="13.42578125" customWidth="1"/>
+    <col min="5" max="12" width="15.375" style="40" customWidth="1"/>
+    <col min="13" max="13" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.25" customWidth="1"/>
+    <col min="25" max="25" width="13.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
@@ -5006,15 +6956,15 @@
   <dimension ref="A1:Y29"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="12" width="15.42578125" style="40" customWidth="1"/>
-    <col min="13" max="13" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.28515625" customWidth="1"/>
-    <col min="25" max="25" width="13.42578125" customWidth="1"/>
+    <col min="5" max="12" width="15.375" style="40" customWidth="1"/>
+    <col min="13" max="13" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.25" customWidth="1"/>
+    <col min="25" max="25" width="13.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
@@ -6285,8 +8235,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="12" max="14" width="14.5703125" customWidth="1"/>
-    <col min="15" max="15" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="14.625" customWidth="1"/>
+    <col min="15" max="15" width="9.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -7065,14 +9015,14 @@
   <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="10" max="10" width="18.28515625" customWidth="1"/>
-    <col min="11" max="13" width="14.5703125" customWidth="1"/>
-    <col min="14" max="14" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.25" customWidth="1"/>
+    <col min="11" max="13" width="14.625" customWidth="1"/>
+    <col min="14" max="14" width="9.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -7297,6 +9247,14 @@
       <c r="H12">
         <v>594</v>
       </c>
+      <c r="I12">
+        <f>SUM(B12:H12)</f>
+        <v>4486</v>
+      </c>
+      <c r="J12">
+        <f>I12*0.05</f>
+        <v>224.3</v>
+      </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -7323,6 +9281,14 @@
       <c r="H13">
         <v>1584</v>
       </c>
+      <c r="I13">
+        <f>SUM(B13:H13)</f>
+        <v>4226</v>
+      </c>
+      <c r="J13">
+        <f>I13*0.16</f>
+        <v>676.16</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -7349,6 +9315,14 @@
       <c r="H14">
         <v>1003</v>
       </c>
+      <c r="I14">
+        <f t="shared" ref="I14:I16" si="0">SUM(B14:H14)</f>
+        <v>2214</v>
+      </c>
+      <c r="J14">
+        <f>I14*0.2</f>
+        <v>442.8</v>
+      </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -7375,6 +9349,14 @@
       <c r="H15">
         <v>225</v>
       </c>
+      <c r="I15">
+        <f t="shared" si="0"/>
+        <v>470</v>
+      </c>
+      <c r="J15">
+        <f>I15*0.22</f>
+        <v>103.4</v>
+      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -7400,6 +9382,14 @@
       </c>
       <c r="H16">
         <v>102</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="0"/>
+        <v>149</v>
+      </c>
+      <c r="J16">
+        <f>I16*0.8</f>
+        <v>119.2</v>
       </c>
     </row>
   </sheetData>
@@ -7421,11 +9411,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="12.5703125" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" customWidth="1"/>
-    <col min="10" max="10" width="18.28515625" customWidth="1"/>
-    <col min="11" max="13" width="14.5703125" customWidth="1"/>
-    <col min="14" max="14" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.625" customWidth="1"/>
+    <col min="8" max="8" width="14.25" customWidth="1"/>
+    <col min="10" max="10" width="18.25" customWidth="1"/>
+    <col min="11" max="13" width="14.625" customWidth="1"/>
+    <col min="14" max="14" width="9.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>